<commit_message>
Change structure of action sell. Selling ship, sell particular percentage of ships, not alwasy all.
</commit_message>
<xml_diff>
--- a/output/ship_rule_charter.xlsx
+++ b/output/ship_rule_charter.xlsx
@@ -383,27 +383,27 @@
         </is>
       </c>
       <c r="B1" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="C1" s="0" t="n">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="D1" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E1" s="0" t="n">
-        <v>400</v>
+        <v>1300</v>
       </c>
       <c r="F1" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>36month charter</t>
         </is>
       </c>
       <c r="G1" s="0" t="n">
-        <v>0.1268109135911205</v>
+        <v>0.02261863089788084</v>
       </c>
       <c r="H1" s="0" t="n">
-        <v>1.503843578328125</v>
+        <v>0.3021609958647269</v>
       </c>
     </row>
     <row r="2">
@@ -413,27 +413,27 @@
         </is>
       </c>
       <c r="B2" s="0" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>400</v>
+        <v>1300</v>
       </c>
       <c r="F2" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>36month charter</t>
         </is>
       </c>
       <c r="G2" s="0" t="n">
-        <v>0.1268109135911205</v>
+        <v>0.02261863089788084</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>1.503843578328125</v>
+        <v>0.3021609958647269</v>
       </c>
     </row>
     <row r="3">
@@ -443,27 +443,27 @@
         </is>
       </c>
       <c r="B3" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>400</v>
+        <v>700</v>
       </c>
       <c r="F3" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>36month charter</t>
         </is>
       </c>
       <c r="G3" s="0" t="n">
-        <v>0.1268109135911205</v>
+        <v>0.02261863089788084</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>1.503843578328125</v>
+        <v>0.3021609958647269</v>
       </c>
     </row>
     <row r="4">
@@ -473,27 +473,27 @@
         </is>
       </c>
       <c r="B4" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>400</v>
+        <v>1300</v>
       </c>
       <c r="F4" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>36month charter</t>
         </is>
       </c>
       <c r="G4" s="0" t="n">
-        <v>0.1268109135911205</v>
+        <v>0.02261863089788084</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>1.503843578328125</v>
+        <v>0.3021609958647269</v>
       </c>
     </row>
     <row r="5">
@@ -503,16 +503,16 @@
         </is>
       </c>
       <c r="B5" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="D5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>650</v>
-      </c>
       <c r="E5" s="0" t="n">
-        <v>700</v>
+        <v>1300</v>
       </c>
       <c r="F5" s="0" t="inlineStr">
         <is>
@@ -520,10 +520,10 @@
         </is>
       </c>
       <c r="G5" s="0" t="n">
-        <v>0.1260630236851297</v>
+        <v>0.02261863089788084</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>1.789230328856783</v>
+        <v>0.3021609958647269</v>
       </c>
     </row>
     <row r="6">
@@ -533,16 +533,16 @@
         </is>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>650</v>
+        <v>200</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>800</v>
+        <v>1300</v>
       </c>
       <c r="F6" s="0" t="inlineStr">
         <is>
@@ -550,10 +550,10 @@
         </is>
       </c>
       <c r="G6" s="0" t="n">
-        <v>0.1260630236851297</v>
+        <v>0.02261863089788084</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>1.789230328856783</v>
+        <v>0.3021609958647269</v>
       </c>
     </row>
     <row r="7">
@@ -563,27 +563,27 @@
         </is>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>900</v>
+        <v>700</v>
       </c>
       <c r="F7" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G7" s="0" t="n">
-        <v>0.09941010642723791</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>0.9278019358072168</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="8">
@@ -593,27 +593,27 @@
         </is>
       </c>
       <c r="B8" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>900</v>
+        <v>700</v>
       </c>
       <c r="F8" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G8" s="0" t="n">
-        <v>0.09941010642723791</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>0.9278019358072168</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="9">
@@ -623,7 +623,7 @@
         </is>
       </c>
       <c r="B9" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>150</v>
@@ -632,18 +632,18 @@
         <v>200</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F9" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G9" s="0" t="n">
-        <v>0.09941010642723791</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>0.9278019358072168</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="10">
@@ -653,27 +653,27 @@
         </is>
       </c>
       <c r="B10" s="0" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>900</v>
+        <v>700</v>
       </c>
       <c r="F10" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G10" s="0" t="n">
-        <v>0.09941010642723791</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>0.9278019358072168</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="11">
@@ -683,27 +683,27 @@
         </is>
       </c>
       <c r="B11" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="F11" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G11" s="0" t="n">
-        <v>0.09941010642723791</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>0.9278019358072168</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="12">
@@ -713,7 +713,7 @@
         </is>
       </c>
       <c r="B12" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>150</v>
@@ -722,18 +722,18 @@
         <v>200</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F12" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G12" s="0" t="n">
-        <v>0.09941010642723791</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>0.9278019358072168</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="13">
@@ -743,27 +743,27 @@
         </is>
       </c>
       <c r="B13" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="F13" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G13" s="0" t="n">
-        <v>0.09941010642723791</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>0.9278019358072168</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="14">
@@ -773,27 +773,27 @@
         </is>
       </c>
       <c r="B14" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="F14" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G14" s="0" t="n">
-        <v>0.09941010642723791</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>0.9278019358072168</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="15">
@@ -803,27 +803,27 @@
         </is>
       </c>
       <c r="B15" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="F15" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G15" s="0" t="n">
-        <v>0.09941010642723791</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>0.9278019358072168</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="16">
@@ -833,27 +833,27 @@
         </is>
       </c>
       <c r="B16" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="F16" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G16" s="0" t="n">
-        <v>0.09941010642723791</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H16" s="0" t="n">
-        <v>0.9278019358072168</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="17">
@@ -863,27 +863,27 @@
         </is>
       </c>
       <c r="B17" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="F17" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G17" s="0" t="n">
-        <v>0.09941010642723791</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H17" s="0" t="n">
-        <v>0.9278019358072168</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="18">
@@ -893,7 +893,7 @@
         </is>
       </c>
       <c r="B18" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>150</v>
@@ -902,18 +902,18 @@
         <v>200</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F18" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G18" s="0" t="n">
-        <v>0.09941010642723791</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H18" s="0" t="n">
-        <v>0.9278019358072168</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="19">
@@ -923,7 +923,7 @@
         </is>
       </c>
       <c r="B19" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>150</v>
@@ -932,18 +932,18 @@
         <v>200</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F19" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G19" s="0" t="n">
-        <v>0.09941010642723791</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H19" s="0" t="n">
-        <v>0.9278019358072168</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="20">
@@ -953,27 +953,27 @@
         </is>
       </c>
       <c r="B20" s="0" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F20" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G20" s="0" t="n">
-        <v>0.09941010642723791</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>0.9278019358072168</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="21">
@@ -983,27 +983,27 @@
         </is>
       </c>
       <c r="B21" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="F21" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G21" s="0" t="n">
-        <v>0.09941010642723791</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>0.9278019358072168</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="22">
@@ -1013,16 +1013,16 @@
         </is>
       </c>
       <c r="B22" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>400</v>
+        <v>700</v>
       </c>
       <c r="F22" s="0" t="inlineStr">
         <is>
@@ -1030,10 +1030,10 @@
         </is>
       </c>
       <c r="G22" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H22" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="23">
@@ -1043,16 +1043,16 @@
         </is>
       </c>
       <c r="B23" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>1500</v>
+        <v>700</v>
       </c>
       <c r="F23" s="0" t="inlineStr">
         <is>
@@ -1060,10 +1060,10 @@
         </is>
       </c>
       <c r="G23" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H23" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="24">
@@ -1073,16 +1073,16 @@
         </is>
       </c>
       <c r="B24" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>400</v>
+        <v>700</v>
       </c>
       <c r="F24" s="0" t="inlineStr">
         <is>
@@ -1090,10 +1090,10 @@
         </is>
       </c>
       <c r="G24" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H24" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="25">
@@ -1103,16 +1103,16 @@
         </is>
       </c>
       <c r="B25" s="0" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>700</v>
+        <v>200</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>1100</v>
+        <v>700</v>
       </c>
       <c r="F25" s="0" t="inlineStr">
         <is>
@@ -1120,10 +1120,10 @@
         </is>
       </c>
       <c r="G25" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H25" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="B26" s="0" t="n">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>150</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>1500</v>
+        <v>700</v>
       </c>
       <c r="F26" s="0" t="inlineStr">
         <is>
@@ -1150,10 +1150,10 @@
         </is>
       </c>
       <c r="G26" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H26" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="27">
@@ -1163,16 +1163,16 @@
         </is>
       </c>
       <c r="B27" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>400</v>
+        <v>700</v>
       </c>
       <c r="F27" s="0" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="G27" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H27" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="28">
@@ -1193,16 +1193,16 @@
         </is>
       </c>
       <c r="B28" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>1500</v>
+        <v>700</v>
       </c>
       <c r="F28" s="0" t="inlineStr">
         <is>
@@ -1210,10 +1210,10 @@
         </is>
       </c>
       <c r="G28" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H28" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="29">
@@ -1223,7 +1223,7 @@
         </is>
       </c>
       <c r="B29" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>150</v>
@@ -1232,7 +1232,7 @@
         <v>200</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="F29" s="0" t="inlineStr">
         <is>
@@ -1240,10 +1240,10 @@
         </is>
       </c>
       <c r="G29" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H29" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="30">
@@ -1253,16 +1253,16 @@
         </is>
       </c>
       <c r="B30" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>400</v>
+        <v>700</v>
       </c>
       <c r="F30" s="0" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         </is>
       </c>
       <c r="G30" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H30" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="31">
@@ -1283,16 +1283,16 @@
         </is>
       </c>
       <c r="B31" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>150</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="F31" s="0" t="inlineStr">
         <is>
@@ -1300,10 +1300,10 @@
         </is>
       </c>
       <c r="G31" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H31" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="32">
@@ -1313,7 +1313,7 @@
         </is>
       </c>
       <c r="B32" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>150</v>
@@ -1322,7 +1322,7 @@
         <v>200</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="F32" s="0" t="inlineStr">
         <is>
@@ -1330,10 +1330,10 @@
         </is>
       </c>
       <c r="G32" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H32" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="33">
@@ -1343,16 +1343,16 @@
         </is>
       </c>
       <c r="B33" s="0" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>700</v>
+        <v>200</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>1100</v>
+        <v>700</v>
       </c>
       <c r="F33" s="0" t="inlineStr">
         <is>
@@ -1360,10 +1360,10 @@
         </is>
       </c>
       <c r="G33" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H33" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="34">
@@ -1373,16 +1373,16 @@
         </is>
       </c>
       <c r="B34" s="0" t="n">
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F34" s="0" t="inlineStr">
         <is>
@@ -1390,10 +1390,10 @@
         </is>
       </c>
       <c r="G34" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H34" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="35">
@@ -1403,7 +1403,7 @@
         </is>
       </c>
       <c r="B35" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>150</v>
@@ -1412,7 +1412,7 @@
         <v>200</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>900</v>
+        <v>700</v>
       </c>
       <c r="F35" s="0" t="inlineStr">
         <is>
@@ -1420,10 +1420,10 @@
         </is>
       </c>
       <c r="G35" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H35" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="36">
@@ -1433,16 +1433,16 @@
         </is>
       </c>
       <c r="B36" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>900</v>
+        <v>200</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>1500</v>
+        <v>700</v>
       </c>
       <c r="F36" s="0" t="inlineStr">
         <is>
@@ -1450,10 +1450,10 @@
         </is>
       </c>
       <c r="G36" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H36" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="37">
@@ -1463,16 +1463,16 @@
         </is>
       </c>
       <c r="B37" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>400</v>
+        <v>700</v>
       </c>
       <c r="F37" s="0" t="inlineStr">
         <is>
@@ -1480,10 +1480,10 @@
         </is>
       </c>
       <c r="G37" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H37" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="38">
@@ -1493,16 +1493,16 @@
         </is>
       </c>
       <c r="B38" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="E38" s="0" t="n">
-        <v>650</v>
+        <v>700</v>
       </c>
       <c r="F38" s="0" t="inlineStr">
         <is>
@@ -1510,10 +1510,10 @@
         </is>
       </c>
       <c r="G38" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H38" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="39">
@@ -1523,16 +1523,16 @@
         </is>
       </c>
       <c r="B39" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>150</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>900</v>
+        <v>700</v>
       </c>
       <c r="F39" s="0" t="inlineStr">
         <is>
@@ -1540,10 +1540,10 @@
         </is>
       </c>
       <c r="G39" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H39" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="40">
@@ -1553,16 +1553,16 @@
         </is>
       </c>
       <c r="B40" s="0" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>700</v>
+        <v>200</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>1100</v>
+        <v>700</v>
       </c>
       <c r="F40" s="0" t="inlineStr">
         <is>
@@ -1570,10 +1570,10 @@
         </is>
       </c>
       <c r="G40" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H40" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="41">
@@ -1583,16 +1583,16 @@
         </is>
       </c>
       <c r="B41" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>150</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>900</v>
+        <v>700</v>
       </c>
       <c r="F41" s="0" t="inlineStr">
         <is>
@@ -1600,10 +1600,10 @@
         </is>
       </c>
       <c r="G41" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H41" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="42">
@@ -1613,16 +1613,16 @@
         </is>
       </c>
       <c r="B42" s="0" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>700</v>
+        <v>200</v>
       </c>
       <c r="E42" s="0" t="n">
-        <v>1100</v>
+        <v>700</v>
       </c>
       <c r="F42" s="0" t="inlineStr">
         <is>
@@ -1630,10 +1630,10 @@
         </is>
       </c>
       <c r="G42" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H42" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="43">
@@ -1643,16 +1643,16 @@
         </is>
       </c>
       <c r="B43" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="E43" s="0" t="n">
-        <v>400</v>
+        <v>700</v>
       </c>
       <c r="F43" s="0" t="inlineStr">
         <is>
@@ -1660,10 +1660,10 @@
         </is>
       </c>
       <c r="G43" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H43" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="44">
@@ -1673,16 +1673,16 @@
         </is>
       </c>
       <c r="B44" s="0" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>700</v>
+        <v>200</v>
       </c>
       <c r="E44" s="0" t="n">
-        <v>1100</v>
+        <v>700</v>
       </c>
       <c r="F44" s="0" t="inlineStr">
         <is>
@@ -1690,10 +1690,10 @@
         </is>
       </c>
       <c r="G44" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H44" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="45">
@@ -1703,16 +1703,16 @@
         </is>
       </c>
       <c r="B45" s="0" t="n">
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E45" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F45" s="0" t="inlineStr">
         <is>
@@ -1720,10 +1720,10 @@
         </is>
       </c>
       <c r="G45" s="0" t="n">
-        <v>0.07598324451406335</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H45" s="0" t="n">
-        <v>1.657762769977424</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="46">
@@ -1733,27 +1733,27 @@
         </is>
       </c>
       <c r="B46" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>650</v>
+        <v>200</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F46" s="0" t="inlineStr">
         <is>
-          <t>3month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G46" s="0" t="n">
-        <v>0.06415353893725806</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H46" s="0" t="n">
-        <v>1.627440241348483</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="47">
@@ -1763,27 +1763,27 @@
         </is>
       </c>
       <c r="B47" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>650</v>
+        <v>200</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F47" s="0" t="inlineStr">
         <is>
-          <t>3month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G47" s="0" t="n">
-        <v>0.06415353893725806</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H47" s="0" t="n">
-        <v>1.627440241348483</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="48">
@@ -1793,27 +1793,27 @@
         </is>
       </c>
       <c r="B48" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>650</v>
+        <v>200</v>
       </c>
       <c r="E48" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F48" s="0" t="inlineStr">
         <is>
-          <t>3month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G48" s="0" t="n">
-        <v>0.06415353893725806</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H48" s="0" t="n">
-        <v>1.627440241348483</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="49">
@@ -1823,27 +1823,27 @@
         </is>
       </c>
       <c r="B49" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>650</v>
+        <v>200</v>
       </c>
       <c r="E49" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F49" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G49" s="0" t="n">
-        <v>0.06120577192304322</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H49" s="0" t="n">
-        <v>1.619927929172494</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="50">
@@ -1853,27 +1853,27 @@
         </is>
       </c>
       <c r="B50" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>650</v>
+        <v>200</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F50" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G50" s="0" t="n">
-        <v>0.06120577192304322</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H50" s="0" t="n">
-        <v>1.619927929172494</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="51">
@@ -1883,27 +1883,27 @@
         </is>
       </c>
       <c r="B51" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>650</v>
+        <v>200</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F51" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G51" s="0" t="n">
-        <v>0.06120577192304322</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H51" s="0" t="n">
-        <v>1.619927929172494</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="52">
@@ -1913,27 +1913,27 @@
         </is>
       </c>
       <c r="B52" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>650</v>
+        <v>200</v>
       </c>
       <c r="E52" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F52" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G52" s="0" t="n">
-        <v>0.06120577192304322</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H52" s="0" t="n">
-        <v>1.619927929172494</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="53">
@@ -1943,27 +1943,27 @@
         </is>
       </c>
       <c r="B53" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>650</v>
+        <v>200</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F53" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G53" s="0" t="n">
-        <v>0.06120577192304322</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H53" s="0" t="n">
-        <v>1.619927929172494</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="54">
@@ -1973,27 +1973,27 @@
         </is>
       </c>
       <c r="B54" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E54" s="0" t="n">
-        <v>650</v>
+        <v>700</v>
       </c>
       <c r="F54" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G54" s="0" t="n">
-        <v>0.04878352242106648</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H54" s="0" t="n">
-        <v>0.8328354284872356</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="55">
@@ -2003,27 +2003,27 @@
         </is>
       </c>
       <c r="B55" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E55" s="0" t="n">
-        <v>650</v>
+        <v>700</v>
       </c>
       <c r="F55" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G55" s="0" t="n">
-        <v>0.04878352242106648</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H55" s="0" t="n">
-        <v>0.8328354284872356</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="56">
@@ -2033,27 +2033,27 @@
         </is>
       </c>
       <c r="B56" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E56" s="0" t="n">
-        <v>650</v>
+        <v>700</v>
       </c>
       <c r="F56" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G56" s="0" t="n">
-        <v>0.04878352242106648</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H56" s="0" t="n">
-        <v>0.8328354284872356</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="57">
@@ -2063,27 +2063,27 @@
         </is>
       </c>
       <c r="B57" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E57" s="0" t="n">
-        <v>650</v>
+        <v>700</v>
       </c>
       <c r="F57" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G57" s="0" t="n">
-        <v>0.04878352242106648</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H57" s="0" t="n">
-        <v>0.8328354284872356</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="58">
@@ -2093,27 +2093,27 @@
         </is>
       </c>
       <c r="B58" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>650</v>
+        <v>200</v>
       </c>
       <c r="E58" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F58" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G58" s="0" t="n">
-        <v>0.04440426158489741</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H58" s="0" t="n">
-        <v>1.577441508485226</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="59">
@@ -2123,27 +2123,27 @@
         </is>
       </c>
       <c r="B59" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>650</v>
+        <v>200</v>
       </c>
       <c r="E59" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F59" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G59" s="0" t="n">
-        <v>0.04440426158489741</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H59" s="0" t="n">
-        <v>1.577441508485226</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="60">
@@ -2153,27 +2153,27 @@
         </is>
       </c>
       <c r="B60" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>650</v>
+        <v>200</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F60" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G60" s="0" t="n">
-        <v>0.04440426158489741</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H60" s="0" t="n">
-        <v>1.577441508485226</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="61">
@@ -2183,27 +2183,27 @@
         </is>
       </c>
       <c r="B61" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>650</v>
+        <v>200</v>
       </c>
       <c r="E61" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F61" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G61" s="0" t="n">
-        <v>0.04440426158489741</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H61" s="0" t="n">
-        <v>1.577441508485226</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="62">
@@ -2213,27 +2213,27 @@
         </is>
       </c>
       <c r="B62" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="C62" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>650</v>
+        <v>200</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F62" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G62" s="0" t="n">
-        <v>0.04440426158489741</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H62" s="0" t="n">
-        <v>1.577441508485226</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="63">
@@ -2243,27 +2243,27 @@
         </is>
       </c>
       <c r="B63" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>550</v>
+        <v>200</v>
       </c>
       <c r="E63" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F63" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G63" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H63" s="0" t="n">
-        <v>1.267489020997062</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="64">
@@ -2273,27 +2273,27 @@
         </is>
       </c>
       <c r="B64" s="0" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="C64" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="E64" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F64" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G64" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H64" s="0" t="n">
-        <v>1.186233448624317</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="65">
@@ -2303,27 +2303,27 @@
         </is>
       </c>
       <c r="B65" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C65" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E65" s="0" t="n">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="F65" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G65" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H65" s="0" t="n">
-        <v>0.9902797084819368</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="66">
@@ -2333,27 +2333,27 @@
         </is>
       </c>
       <c r="B66" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C66" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E66" s="0" t="n">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="F66" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G66" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H66" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="67">
@@ -2363,27 +2363,27 @@
         </is>
       </c>
       <c r="B67" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C67" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E67" s="0" t="n">
-        <v>1500</v>
+        <v>700</v>
       </c>
       <c r="F67" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G67" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H67" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="68">
@@ -2393,7 +2393,7 @@
         </is>
       </c>
       <c r="B68" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C68" s="0" t="n">
         <v>150</v>
@@ -2402,18 +2402,18 @@
         <v>200</v>
       </c>
       <c r="E68" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F68" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G68" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H68" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="69">
@@ -2423,10 +2423,10 @@
         </is>
       </c>
       <c r="B69" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C69" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>200</v>
@@ -2436,14 +2436,14 @@
       </c>
       <c r="F69" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G69" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H69" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="70">
@@ -2453,10 +2453,10 @@
         </is>
       </c>
       <c r="B70" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C70" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>200</v>
@@ -2466,14 +2466,14 @@
       </c>
       <c r="F70" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G70" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H70" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="71">
@@ -2483,27 +2483,27 @@
         </is>
       </c>
       <c r="B71" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C71" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>550</v>
+        <v>200</v>
       </c>
       <c r="E71" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F71" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G71" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H71" s="0" t="n">
-        <v>1.267489020997062</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="72">
@@ -2513,27 +2513,27 @@
         </is>
       </c>
       <c r="B72" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C72" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E72" s="0" t="n">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="F72" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G72" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H72" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="73">
@@ -2543,27 +2543,27 @@
         </is>
       </c>
       <c r="B73" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C73" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E73" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F73" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G73" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H73" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="74">
@@ -2573,27 +2573,27 @@
         </is>
       </c>
       <c r="B74" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C74" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D74" s="0" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="E74" s="0" t="n">
-        <v>650</v>
+        <v>700</v>
       </c>
       <c r="F74" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G74" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H74" s="0" t="n">
-        <v>1.10558090894286</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="75">
@@ -2603,27 +2603,27 @@
         </is>
       </c>
       <c r="B75" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C75" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D75" s="0" t="n">
-        <v>550</v>
+        <v>200</v>
       </c>
       <c r="E75" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F75" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G75" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H75" s="0" t="n">
-        <v>1.267489020997062</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="76">
@@ -2633,27 +2633,27 @@
         </is>
       </c>
       <c r="B76" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C76" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E76" s="0" t="n">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="F76" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G76" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H76" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="77">
@@ -2663,10 +2663,10 @@
         </is>
       </c>
       <c r="B77" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C77" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D77" s="0" t="n">
         <v>200</v>
@@ -2676,14 +2676,14 @@
       </c>
       <c r="F77" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G77" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H77" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="78">
@@ -2693,10 +2693,10 @@
         </is>
       </c>
       <c r="B78" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C78" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D78" s="0" t="n">
         <v>200</v>
@@ -2706,14 +2706,14 @@
       </c>
       <c r="F78" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G78" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H78" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="79">
@@ -2723,27 +2723,27 @@
         </is>
       </c>
       <c r="B79" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C79" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>550</v>
+        <v>200</v>
       </c>
       <c r="E79" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F79" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G79" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H79" s="0" t="n">
-        <v>1.267489020997062</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="80">
@@ -2753,10 +2753,10 @@
         </is>
       </c>
       <c r="B80" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C80" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D80" s="0" t="n">
         <v>200</v>
@@ -2766,14 +2766,14 @@
       </c>
       <c r="F80" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G80" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H80" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="81">
@@ -2783,27 +2783,27 @@
         </is>
       </c>
       <c r="B81" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C81" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>550</v>
+        <v>200</v>
       </c>
       <c r="E81" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F81" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G81" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H81" s="0" t="n">
-        <v>1.267489020997062</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="82">
@@ -2813,27 +2813,27 @@
         </is>
       </c>
       <c r="B82" s="0" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="C82" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="D82" s="0" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="E82" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F82" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G82" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H82" s="0" t="n">
-        <v>1.028727855284902</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="83">
@@ -2843,27 +2843,27 @@
         </is>
       </c>
       <c r="B83" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C83" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D83" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E83" s="0" t="n">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="F83" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G83" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H83" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="84">
@@ -2873,27 +2873,27 @@
         </is>
       </c>
       <c r="B84" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C84" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D84" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E84" s="0" t="n">
-        <v>1500</v>
+        <v>700</v>
       </c>
       <c r="F84" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G84" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H84" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="85">
@@ -2903,27 +2903,27 @@
         </is>
       </c>
       <c r="B85" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C85" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D85" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E85" s="0" t="n">
-        <v>1500</v>
+        <v>700</v>
       </c>
       <c r="F85" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G85" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H85" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="86">
@@ -2933,27 +2933,27 @@
         </is>
       </c>
       <c r="B86" s="0" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="C86" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="D86" s="0" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F86" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G86" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H86" s="0" t="n">
-        <v>1.186233448624317</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="87">
@@ -2963,27 +2963,27 @@
         </is>
       </c>
       <c r="B87" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C87" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D87" s="0" t="n">
-        <v>550</v>
+        <v>200</v>
       </c>
       <c r="E87" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F87" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G87" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H87" s="0" t="n">
-        <v>1.267489020997062</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="88">
@@ -2993,27 +2993,27 @@
         </is>
       </c>
       <c r="B88" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C88" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D88" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E88" s="0" t="n">
-        <v>1500</v>
+        <v>700</v>
       </c>
       <c r="F88" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G88" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H88" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="89">
@@ -3023,27 +3023,27 @@
         </is>
       </c>
       <c r="B89" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C89" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D89" s="0" t="n">
-        <v>550</v>
+        <v>200</v>
       </c>
       <c r="E89" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F89" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G89" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H89" s="0" t="n">
-        <v>1.267489020997062</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="90">
@@ -3053,7 +3053,7 @@
         </is>
       </c>
       <c r="B90" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C90" s="0" t="n">
         <v>150</v>
@@ -3062,18 +3062,18 @@
         <v>200</v>
       </c>
       <c r="E90" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F90" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G90" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H90" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="91">
@@ -3083,7 +3083,7 @@
         </is>
       </c>
       <c r="B91" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C91" s="0" t="n">
         <v>150</v>
@@ -3092,18 +3092,18 @@
         <v>200</v>
       </c>
       <c r="E91" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F91" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G91" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H91" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="92">
@@ -3113,27 +3113,27 @@
         </is>
       </c>
       <c r="B92" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C92" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D92" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E92" s="0" t="n">
-        <v>1500</v>
+        <v>700</v>
       </c>
       <c r="F92" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G92" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H92" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="93">
@@ -3143,27 +3143,27 @@
         </is>
       </c>
       <c r="B93" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C93" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D93" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E93" s="0" t="n">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="F93" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G93" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H93" s="0" t="n">
-        <v>0.9902797084819368</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="94">
@@ -3173,27 +3173,27 @@
         </is>
       </c>
       <c r="B94" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C94" s="0" t="n">
         <v>150</v>
       </c>
       <c r="D94" s="0" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="E94" s="0" t="n">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="F94" s="0" t="inlineStr">
         <is>
-          <t>3month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G94" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H94" s="0" t="n">
-        <v>1.272635218131662</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="95">
@@ -3203,27 +3203,27 @@
         </is>
       </c>
       <c r="B95" s="0" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="C95" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="D95" s="0" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="E95" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F95" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G95" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H95" s="0" t="n">
-        <v>1.028727855284902</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="96">
@@ -3233,27 +3233,27 @@
         </is>
       </c>
       <c r="B96" s="0" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="C96" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="D96" s="0" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="E96" s="0" t="n">
         <v>700</v>
       </c>
       <c r="F96" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G96" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H96" s="0" t="n">
-        <v>1.028727855284902</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="97">
@@ -3263,10 +3263,10 @@
         </is>
       </c>
       <c r="B97" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C97" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D97" s="0" t="n">
         <v>200</v>
@@ -3276,14 +3276,14 @@
       </c>
       <c r="F97" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G97" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H97" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="98">
@@ -3293,27 +3293,27 @@
         </is>
       </c>
       <c r="B98" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C98" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D98" s="0" t="n">
-        <v>550</v>
+        <v>200</v>
       </c>
       <c r="E98" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F98" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G98" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H98" s="0" t="n">
-        <v>1.267489020997062</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="99">
@@ -3323,27 +3323,27 @@
         </is>
       </c>
       <c r="B99" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C99" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D99" s="0" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="E99" s="0" t="n">
-        <v>650</v>
+        <v>700</v>
       </c>
       <c r="F99" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G99" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H99" s="0" t="n">
-        <v>1.10558090894286</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
     <row r="100">
@@ -3353,27 +3353,27 @@
         </is>
       </c>
       <c r="B100" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C100" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D100" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E100" s="0" t="n">
-        <v>1500</v>
+        <v>700</v>
       </c>
       <c r="F100" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G100" s="0" t="n">
-        <v>0</v>
+        <v>-0.0723458748753751</v>
       </c>
       <c r="H100" s="0" t="n">
-        <v>0.9372160810466608</v>
+        <v>0.3026602104177025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set initial number of ships as 100. Modify idle_rate.If sell some ships, then idle_rate decrease.
</commit_message>
<xml_diff>
--- a/output/ship_rule_charter.xlsx
+++ b/output/ship_rule_charter.xlsx
@@ -383,27 +383,27 @@
         </is>
       </c>
       <c r="B1" s="0" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C1" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D1" s="0" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E1" s="0" t="n">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="F1" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G1" s="0" t="n">
-        <v>0.2375982127893829</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H1" s="0" t="n">
-        <v>1.105645159451233</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="2">
@@ -413,27 +413,27 @@
         </is>
       </c>
       <c r="B2" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>300</v>
+        <v>1500</v>
       </c>
       <c r="F2" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G2" s="0" t="n">
-        <v>0.2375982127893829</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>1.105645159451233</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="3">
@@ -443,27 +443,27 @@
         </is>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="F3" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G3" s="0" t="n">
-        <v>0.2375982127893829</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>1.105645159451233</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="4">
@@ -473,27 +473,27 @@
         </is>
       </c>
       <c r="B4" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>300</v>
+        <v>1500</v>
       </c>
       <c r="F4" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G4" s="0" t="n">
-        <v>0.2375982127893829</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>1.105645159451233</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="5">
@@ -503,27 +503,27 @@
         </is>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>300</v>
+        <v>1500</v>
       </c>
       <c r="F5" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G5" s="0" t="n">
-        <v>0.2375982127893829</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>1.105645159451233</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="6">
@@ -533,27 +533,27 @@
         </is>
       </c>
       <c r="B6" s="0" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>110</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="F6" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G6" s="0" t="n">
-        <v>0.2375982127893829</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>1.105645159451233</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="7">
@@ -563,27 +563,27 @@
         </is>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>300</v>
+        <v>1500</v>
       </c>
       <c r="F7" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G7" s="0" t="n">
-        <v>0.2375982127893829</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>1.105645159451233</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="8">
@@ -593,27 +593,27 @@
         </is>
       </c>
       <c r="B8" s="0" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>300</v>
+        <v>1300</v>
       </c>
       <c r="F8" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G8" s="0" t="n">
-        <v>0.2375982127893829</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>1.105645159451233</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="9">
@@ -623,27 +623,27 @@
         </is>
       </c>
       <c r="B9" s="0" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="F9" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G9" s="0" t="n">
-        <v>0.2375982127893829</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>1.105645159451233</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="10">
@@ -653,27 +653,27 @@
         </is>
       </c>
       <c r="B10" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>300</v>
+        <v>1500</v>
       </c>
       <c r="F10" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G10" s="0" t="n">
-        <v>0.2375982127893829</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>1.105645159451233</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="11">
@@ -686,24 +686,24 @@
         <v>0</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="F11" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G11" s="0" t="n">
-        <v>0.2375982127893829</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>1.105645159451233</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="12">
@@ -713,27 +713,27 @@
         </is>
       </c>
       <c r="B12" s="0" t="n">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="F12" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G12" s="0" t="n">
-        <v>0.2260937814008106</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>1.080521908518215</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="13">
@@ -743,27 +743,27 @@
         </is>
       </c>
       <c r="B13" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>400</v>
+        <v>550</v>
       </c>
       <c r="F13" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G13" s="0" t="n">
-        <v>0.2260937814008106</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>1.080521908518215</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="14">
@@ -773,27 +773,27 @@
         </is>
       </c>
       <c r="B14" s="0" t="n">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="F14" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G14" s="0" t="n">
-        <v>0.2260937814008106</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>1.080521908518215</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="15">
@@ -803,27 +803,27 @@
         </is>
       </c>
       <c r="B15" s="0" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>110</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="F15" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G15" s="0" t="n">
-        <v>0.2260937814008106</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>1.080521908518215</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="16">
@@ -836,24 +836,24 @@
         <v>10</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="F16" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G16" s="0" t="n">
-        <v>0.2260937814008106</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H16" s="0" t="n">
-        <v>1.080521908518215</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="17">
@@ -863,27 +863,27 @@
         </is>
       </c>
       <c r="B17" s="0" t="n">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>400</v>
+        <v>1500</v>
       </c>
       <c r="F17" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G17" s="0" t="n">
-        <v>0.2260937814008106</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H17" s="0" t="n">
-        <v>1.080521908518215</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="18">
@@ -893,27 +893,27 @@
         </is>
       </c>
       <c r="B18" s="0" t="n">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="F18" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G18" s="0" t="n">
-        <v>0.2260937814008106</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H18" s="0" t="n">
-        <v>1.080521908518215</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="19">
@@ -923,16 +923,16 @@
         </is>
       </c>
       <c r="B19" s="0" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>600</v>
+        <v>800</v>
       </c>
       <c r="F19" s="0" t="inlineStr">
         <is>
@@ -940,10 +940,10 @@
         </is>
       </c>
       <c r="G19" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H19" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="20">
@@ -953,16 +953,16 @@
         </is>
       </c>
       <c r="B20" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="F20" s="0" t="inlineStr">
         <is>
@@ -970,10 +970,10 @@
         </is>
       </c>
       <c r="G20" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="21">
@@ -983,16 +983,16 @@
         </is>
       </c>
       <c r="B21" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>100</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>200</v>
+        <v>1500</v>
       </c>
       <c r="F21" s="0" t="inlineStr">
         <is>
@@ -1000,10 +1000,10 @@
         </is>
       </c>
       <c r="G21" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="22">
@@ -1013,13 +1013,13 @@
         </is>
       </c>
       <c r="B22" s="0" t="n">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>600</v>
@@ -1030,10 +1030,10 @@
         </is>
       </c>
       <c r="G22" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H22" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="23">
@@ -1043,16 +1043,16 @@
         </is>
       </c>
       <c r="B23" s="0" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>200</v>
+        <v>1500</v>
       </c>
       <c r="F23" s="0" t="inlineStr">
         <is>
@@ -1060,10 +1060,10 @@
         </is>
       </c>
       <c r="G23" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H23" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="24">
@@ -1073,16 +1073,16 @@
         </is>
       </c>
       <c r="B24" s="0" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="F24" s="0" t="inlineStr">
         <is>
@@ -1090,10 +1090,10 @@
         </is>
       </c>
       <c r="G24" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H24" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="25">
@@ -1103,16 +1103,16 @@
         </is>
       </c>
       <c r="B25" s="0" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>1100</v>
+        <v>650</v>
       </c>
       <c r="F25" s="0" t="inlineStr">
         <is>
@@ -1120,10 +1120,10 @@
         </is>
       </c>
       <c r="G25" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H25" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="26">
@@ -1133,16 +1133,16 @@
         </is>
       </c>
       <c r="B26" s="0" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="F26" s="0" t="inlineStr">
         <is>
@@ -1150,10 +1150,10 @@
         </is>
       </c>
       <c r="G26" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H26" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="27">
@@ -1163,16 +1163,16 @@
         </is>
       </c>
       <c r="B27" s="0" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="F27" s="0" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="G27" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H27" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="28">
@@ -1193,16 +1193,16 @@
         </is>
       </c>
       <c r="B28" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>200</v>
+        <v>1500</v>
       </c>
       <c r="F28" s="0" t="inlineStr">
         <is>
@@ -1210,10 +1210,10 @@
         </is>
       </c>
       <c r="G28" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H28" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="29">
@@ -1226,13 +1226,13 @@
         <v>0</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="F29" s="0" t="inlineStr">
         <is>
@@ -1240,10 +1240,10 @@
         </is>
       </c>
       <c r="G29" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H29" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="30">
@@ -1256,13 +1256,13 @@
         <v>0</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="F30" s="0" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         </is>
       </c>
       <c r="G30" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H30" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="31">
@@ -1283,13 +1283,13 @@
         </is>
       </c>
       <c r="B31" s="0" t="n">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>600</v>
@@ -1300,10 +1300,10 @@
         </is>
       </c>
       <c r="G31" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H31" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="32">
@@ -1313,16 +1313,16 @@
         </is>
       </c>
       <c r="B32" s="0" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="F32" s="0" t="inlineStr">
         <is>
@@ -1330,10 +1330,10 @@
         </is>
       </c>
       <c r="G32" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H32" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="33">
@@ -1343,16 +1343,16 @@
         </is>
       </c>
       <c r="B33" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>100</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>200</v>
+        <v>1500</v>
       </c>
       <c r="F33" s="0" t="inlineStr">
         <is>
@@ -1360,10 +1360,10 @@
         </is>
       </c>
       <c r="G33" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H33" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="34">
@@ -1373,16 +1373,16 @@
         </is>
       </c>
       <c r="B34" s="0" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="F34" s="0" t="inlineStr">
         <is>
@@ -1390,10 +1390,10 @@
         </is>
       </c>
       <c r="G34" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H34" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="35">
@@ -1403,16 +1403,16 @@
         </is>
       </c>
       <c r="B35" s="0" t="n">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>600</v>
+        <v>650</v>
       </c>
       <c r="F35" s="0" t="inlineStr">
         <is>
@@ -1420,10 +1420,10 @@
         </is>
       </c>
       <c r="G35" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H35" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="36">
@@ -1433,16 +1433,16 @@
         </is>
       </c>
       <c r="B36" s="0" t="n">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>600</v>
+        <v>650</v>
       </c>
       <c r="F36" s="0" t="inlineStr">
         <is>
@@ -1450,10 +1450,10 @@
         </is>
       </c>
       <c r="G36" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H36" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="37">
@@ -1463,16 +1463,16 @@
         </is>
       </c>
       <c r="B37" s="0" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>200</v>
+        <v>800</v>
       </c>
       <c r="F37" s="0" t="inlineStr">
         <is>
@@ -1480,10 +1480,10 @@
         </is>
       </c>
       <c r="G37" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H37" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="38">
@@ -1493,16 +1493,16 @@
         </is>
       </c>
       <c r="B38" s="0" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="E38" s="0" t="n">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="F38" s="0" t="inlineStr">
         <is>
@@ -1510,10 +1510,10 @@
         </is>
       </c>
       <c r="G38" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H38" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="39">
@@ -1523,16 +1523,16 @@
         </is>
       </c>
       <c r="B39" s="0" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>150</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>400</v>
+        <v>900</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>600</v>
+        <v>1500</v>
       </c>
       <c r="F39" s="0" t="inlineStr">
         <is>
@@ -1540,10 +1540,10 @@
         </is>
       </c>
       <c r="G39" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H39" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="40">
@@ -1553,16 +1553,16 @@
         </is>
       </c>
       <c r="B40" s="0" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="F40" s="0" t="inlineStr">
         <is>
@@ -1570,10 +1570,10 @@
         </is>
       </c>
       <c r="G40" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H40" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="41">
@@ -1583,16 +1583,16 @@
         </is>
       </c>
       <c r="B41" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="F41" s="0" t="inlineStr">
         <is>
@@ -1600,10 +1600,10 @@
         </is>
       </c>
       <c r="G41" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H41" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="42">
@@ -1613,16 +1613,16 @@
         </is>
       </c>
       <c r="B42" s="0" t="n">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>150</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="E42" s="0" t="n">
-        <v>600</v>
+        <v>550</v>
       </c>
       <c r="F42" s="0" t="inlineStr">
         <is>
@@ -1630,10 +1630,10 @@
         </is>
       </c>
       <c r="G42" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H42" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="43">
@@ -1643,16 +1643,16 @@
         </is>
       </c>
       <c r="B43" s="0" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="E43" s="0" t="n">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="F43" s="0" t="inlineStr">
         <is>
@@ -1660,10 +1660,10 @@
         </is>
       </c>
       <c r="G43" s="0" t="n">
-        <v>0.2256006187247376</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H43" s="0" t="n">
-        <v>1.148878896610119</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="44">
@@ -1673,27 +1673,27 @@
         </is>
       </c>
       <c r="B44" s="0" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>150</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E44" s="0" t="n">
-        <v>800</v>
+        <v>550</v>
       </c>
       <c r="F44" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G44" s="0" t="n">
-        <v>0.2252698520054266</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H44" s="0" t="n">
-        <v>1.142138023174508</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="45">
@@ -1703,27 +1703,27 @@
         </is>
       </c>
       <c r="B45" s="0" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E45" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="F45" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G45" s="0" t="n">
-        <v>0.2252698520054266</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H45" s="0" t="n">
-        <v>1.142138023174508</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="46">
@@ -1733,27 +1733,27 @@
         </is>
       </c>
       <c r="B46" s="0" t="n">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E46" s="0" t="n">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="F46" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G46" s="0" t="n">
-        <v>0.2252698520054266</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H46" s="0" t="n">
-        <v>1.142138023174508</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="47">
@@ -1763,27 +1763,27 @@
         </is>
       </c>
       <c r="B47" s="0" t="n">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="E47" s="0" t="n">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="F47" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G47" s="0" t="n">
-        <v>0.2245996401518356</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H47" s="0" t="n">
-        <v>1.147913963553311</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="48">
@@ -1793,27 +1793,27 @@
         </is>
       </c>
       <c r="B48" s="0" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="E48" s="0" t="n">
-        <v>800</v>
+        <v>1500</v>
       </c>
       <c r="F48" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G48" s="0" t="n">
-        <v>0.2245996401518356</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H48" s="0" t="n">
-        <v>1.147913963553311</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="49">
@@ -1823,27 +1823,27 @@
         </is>
       </c>
       <c r="B49" s="0" t="n">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>600</v>
+        <v>750</v>
       </c>
       <c r="E49" s="0" t="n">
-        <v>800</v>
+        <v>1500</v>
       </c>
       <c r="F49" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G49" s="0" t="n">
-        <v>0.2245996401518356</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H49" s="0" t="n">
-        <v>1.147913963553311</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="50">
@@ -1853,27 +1853,27 @@
         </is>
       </c>
       <c r="B50" s="0" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>130</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="E50" s="0" t="n">
-        <v>800</v>
+        <v>1500</v>
       </c>
       <c r="F50" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G50" s="0" t="n">
-        <v>0.2245996401518356</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H50" s="0" t="n">
-        <v>1.147913963553311</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="51">
@@ -1883,27 +1883,27 @@
         </is>
       </c>
       <c r="B51" s="0" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E51" s="0" t="n">
-        <v>650</v>
+        <v>1000</v>
       </c>
       <c r="F51" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G51" s="0" t="n">
-        <v>0.2243432872109393</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H51" s="0" t="n">
-        <v>1.1303824407048</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="52">
@@ -1913,27 +1913,27 @@
         </is>
       </c>
       <c r="B52" s="0" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E52" s="0" t="n">
-        <v>650</v>
+        <v>1100</v>
       </c>
       <c r="F52" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G52" s="0" t="n">
-        <v>0.2243432872109393</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H52" s="0" t="n">
-        <v>1.1303824407048</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="53">
@@ -1943,7 +1943,7 @@
         </is>
       </c>
       <c r="B53" s="0" t="n">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="C53" s="0" t="n">
         <v>130</v>
@@ -1952,18 +1952,18 @@
         <v>300</v>
       </c>
       <c r="E53" s="0" t="n">
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="F53" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="G53" s="0" t="n">
-        <v>0.2240380028169702</v>
+        <v>1.1327699761026</v>
       </c>
       <c r="H53" s="0" t="n">
-        <v>0.991766847860993</v>
+        <v>0.1925132539155783</v>
       </c>
     </row>
     <row r="54">
@@ -1973,27 +1973,27 @@
         </is>
       </c>
       <c r="B54" s="0" t="n">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E54" s="0" t="n">
-        <v>650</v>
+        <v>550</v>
       </c>
       <c r="F54" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>3month charter</t>
         </is>
       </c>
       <c r="G54" s="0" t="n">
-        <v>0.2200428081575873</v>
+        <v>1.043952471110754</v>
       </c>
       <c r="H54" s="0" t="n">
-        <v>1.13088841381744</v>
+        <v>0.1800402363869646</v>
       </c>
     </row>
     <row r="55">
@@ -2003,16 +2003,16 @@
         </is>
       </c>
       <c r="B55" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>130</v>
+        <v>50</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="E55" s="0" t="n">
-        <v>400</v>
+        <v>550</v>
       </c>
       <c r="F55" s="0" t="inlineStr">
         <is>
@@ -2020,10 +2020,10 @@
         </is>
       </c>
       <c r="G55" s="0" t="n">
-        <v>0.2178918809433483</v>
+        <v>1.043952471110754</v>
       </c>
       <c r="H55" s="0" t="n">
-        <v>1.13711965946434</v>
+        <v>0.1800402363869646</v>
       </c>
     </row>
     <row r="56">
@@ -2036,13 +2036,13 @@
         <v>20</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>130</v>
+        <v>50</v>
       </c>
       <c r="D56" s="0" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="E56" s="0" t="n">
-        <v>400</v>
+        <v>550</v>
       </c>
       <c r="F56" s="0" t="inlineStr">
         <is>
@@ -2050,10 +2050,10 @@
         </is>
       </c>
       <c r="G56" s="0" t="n">
-        <v>0.2178918809433483</v>
+        <v>1.043952471110754</v>
       </c>
       <c r="H56" s="0" t="n">
-        <v>1.13711965946434</v>
+        <v>0.1800402363869646</v>
       </c>
     </row>
     <row r="57">
@@ -2063,13 +2063,13 @@
         </is>
       </c>
       <c r="B57" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E57" s="0" t="n">
         <v>550</v>
@@ -2080,10 +2080,10 @@
         </is>
       </c>
       <c r="G57" s="0" t="n">
-        <v>0.2176542698479519</v>
+        <v>1.043952471110754</v>
       </c>
       <c r="H57" s="0" t="n">
-        <v>1.138280450953648</v>
+        <v>0.1800402363869646</v>
       </c>
     </row>
     <row r="58">
@@ -2093,16 +2093,16 @@
         </is>
       </c>
       <c r="B58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C58" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="C58" s="0" t="n">
-        <v>110</v>
-      </c>
       <c r="D58" s="0" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="E58" s="0" t="n">
-        <v>800</v>
+        <v>550</v>
       </c>
       <c r="F58" s="0" t="inlineStr">
         <is>
@@ -2110,10 +2110,10 @@
         </is>
       </c>
       <c r="G58" s="0" t="n">
-        <v>0.2091882290144071</v>
+        <v>1.043952471110754</v>
       </c>
       <c r="H58" s="0" t="n">
-        <v>1.104713658806039</v>
+        <v>0.1800402363869646</v>
       </c>
     </row>
     <row r="59">
@@ -2123,16 +2123,16 @@
         </is>
       </c>
       <c r="B59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C59" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="C59" s="0" t="n">
-        <v>100</v>
-      </c>
       <c r="D59" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E59" s="0" t="n">
-        <v>800</v>
+        <v>550</v>
       </c>
       <c r="F59" s="0" t="inlineStr">
         <is>
@@ -2140,10 +2140,10 @@
         </is>
       </c>
       <c r="G59" s="0" t="n">
-        <v>0.2084351102964472</v>
+        <v>1.043952471110754</v>
       </c>
       <c r="H59" s="0" t="n">
-        <v>1.122497579313701</v>
+        <v>0.1800402363869646</v>
       </c>
     </row>
     <row r="60">
@@ -2153,16 +2153,16 @@
         </is>
       </c>
       <c r="B60" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C60" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="C60" s="0" t="n">
-        <v>110</v>
-      </c>
       <c r="D60" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E60" s="0" t="n">
-        <v>800</v>
+        <v>550</v>
       </c>
       <c r="F60" s="0" t="inlineStr">
         <is>
@@ -2170,10 +2170,10 @@
         </is>
       </c>
       <c r="G60" s="0" t="n">
-        <v>0.2084351102964472</v>
+        <v>1.043952471110754</v>
       </c>
       <c r="H60" s="0" t="n">
-        <v>1.122497579313701</v>
+        <v>0.1800402363869646</v>
       </c>
     </row>
     <row r="61">
@@ -2183,27 +2183,27 @@
         </is>
       </c>
       <c r="B61" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C61" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="C61" s="0" t="n">
-        <v>110</v>
-      </c>
       <c r="D61" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E61" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="F61" s="0" t="inlineStr">
         <is>
-          <t>3month charter</t>
+          <t>6month charter</t>
         </is>
       </c>
       <c r="G61" s="0" t="n">
-        <v>0.2084351102964472</v>
+        <v>1.03419216018902</v>
       </c>
       <c r="H61" s="0" t="n">
-        <v>1.122497579313701</v>
+        <v>0.206665133825527</v>
       </c>
     </row>
     <row r="62">
@@ -2213,27 +2213,27 @@
         </is>
       </c>
       <c r="B62" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C62" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="C62" s="0" t="n">
-        <v>100</v>
-      </c>
       <c r="D62" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E62" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="F62" s="0" t="inlineStr">
         <is>
-          <t>3month charter</t>
+          <t>6month charter</t>
         </is>
       </c>
       <c r="G62" s="0" t="n">
-        <v>0.2084351102964472</v>
+        <v>1.03419216018902</v>
       </c>
       <c r="H62" s="0" t="n">
-        <v>1.122497579313701</v>
+        <v>0.206665133825527</v>
       </c>
     </row>
     <row r="63">
@@ -2243,27 +2243,27 @@
         </is>
       </c>
       <c r="B63" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C63" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="C63" s="0" t="n">
-        <v>110</v>
-      </c>
       <c r="D63" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E63" s="0" t="n">
-        <v>800</v>
+        <v>650</v>
       </c>
       <c r="F63" s="0" t="inlineStr">
         <is>
-          <t>3month charter</t>
+          <t>6month charter</t>
         </is>
       </c>
       <c r="G63" s="0" t="n">
-        <v>0.2084351102964472</v>
+        <v>1.019012132433608</v>
       </c>
       <c r="H63" s="0" t="n">
-        <v>1.122497579313701</v>
+        <v>0.1954469684487564</v>
       </c>
     </row>
     <row r="64">
@@ -2273,16 +2273,16 @@
         </is>
       </c>
       <c r="B64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C64" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="C64" s="0" t="n">
-        <v>110</v>
-      </c>
       <c r="D64" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E64" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="F64" s="0" t="inlineStr">
         <is>
@@ -2290,10 +2290,10 @@
         </is>
       </c>
       <c r="G64" s="0" t="n">
-        <v>0.2084351102964472</v>
+        <v>0.9750367964684676</v>
       </c>
       <c r="H64" s="0" t="n">
-        <v>1.122497579313701</v>
+        <v>0.154116020643822</v>
       </c>
     </row>
     <row r="65">
@@ -2303,16 +2303,16 @@
         </is>
       </c>
       <c r="B65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C65" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="C65" s="0" t="n">
-        <v>100</v>
-      </c>
       <c r="D65" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E65" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="F65" s="0" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="G65" s="0" t="n">
-        <v>0.2084351102964472</v>
+        <v>0.9750367964684676</v>
       </c>
       <c r="H65" s="0" t="n">
-        <v>1.122497579313701</v>
+        <v>0.154116020643822</v>
       </c>
     </row>
     <row r="66">
@@ -2333,27 +2333,27 @@
         </is>
       </c>
       <c r="B66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C66" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="C66" s="0" t="n">
-        <v>110</v>
-      </c>
       <c r="D66" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E66" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="F66" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>3month charter</t>
         </is>
       </c>
       <c r="G66" s="0" t="n">
-        <v>0.1941235761238311</v>
+        <v>0.9750367964684676</v>
       </c>
       <c r="H66" s="0" t="n">
-        <v>1.070026426722869</v>
+        <v>0.154116020643822</v>
       </c>
     </row>
     <row r="67">
@@ -2363,27 +2363,27 @@
         </is>
       </c>
       <c r="B67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C67" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="C67" s="0" t="n">
-        <v>100</v>
-      </c>
       <c r="D67" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E67" s="0" t="n">
-        <v>900</v>
+        <v>600</v>
       </c>
       <c r="F67" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>3month charter</t>
         </is>
       </c>
       <c r="G67" s="0" t="n">
-        <v>0.1934268552445403</v>
+        <v>0.9750367964684676</v>
       </c>
       <c r="H67" s="0" t="n">
-        <v>1.067561528292186</v>
+        <v>0.154116020643822</v>
       </c>
     </row>
     <row r="68">
@@ -2393,27 +2393,27 @@
         </is>
       </c>
       <c r="B68" s="0" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C68" s="0" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D68" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E68" s="0" t="n">
-        <v>900</v>
+        <v>750</v>
       </c>
       <c r="F68" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>3month charter</t>
         </is>
       </c>
       <c r="G68" s="0" t="n">
-        <v>0.1934268552445403</v>
+        <v>0.9247398908928383</v>
       </c>
       <c r="H68" s="0" t="n">
-        <v>1.067561528292186</v>
+        <v>0.2508544423458689</v>
       </c>
     </row>
     <row r="69">
@@ -2423,27 +2423,27 @@
         </is>
       </c>
       <c r="B69" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C69" s="0" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="D69" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E69" s="0" t="n">
-        <v>900</v>
+        <v>600</v>
       </c>
       <c r="F69" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>3month charter</t>
         </is>
       </c>
       <c r="G69" s="0" t="n">
-        <v>0.1934268552445403</v>
+        <v>0.9194632804429046</v>
       </c>
       <c r="H69" s="0" t="n">
-        <v>1.067561528292186</v>
+        <v>0.200838108426977</v>
       </c>
     </row>
     <row r="70">
@@ -2453,27 +2453,27 @@
         </is>
       </c>
       <c r="B70" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C70" s="0" t="n">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="D70" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E70" s="0" t="n">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="F70" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>3month charter</t>
         </is>
       </c>
       <c r="G70" s="0" t="n">
-        <v>0.1917782300424008</v>
+        <v>0.9194632804429046</v>
       </c>
       <c r="H70" s="0" t="n">
-        <v>1.062111722117706</v>
+        <v>0.200838108426977</v>
       </c>
     </row>
     <row r="71">
@@ -2483,27 +2483,27 @@
         </is>
       </c>
       <c r="B71" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C71" s="0" t="n">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E71" s="0" t="n">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="F71" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>3month charter</t>
         </is>
       </c>
       <c r="G71" s="0" t="n">
-        <v>0.1917782300424008</v>
+        <v>0.9194632804429046</v>
       </c>
       <c r="H71" s="0" t="n">
-        <v>1.062111722117706</v>
+        <v>0.200838108426977</v>
       </c>
     </row>
     <row r="72">
@@ -2513,27 +2513,27 @@
         </is>
       </c>
       <c r="B72" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C72" s="0" t="n">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="D72" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E72" s="0" t="n">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="F72" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>3month charter</t>
         </is>
       </c>
       <c r="G72" s="0" t="n">
-        <v>0.1917782300424008</v>
+        <v>0.9194632804429046</v>
       </c>
       <c r="H72" s="0" t="n">
-        <v>1.062111722117706</v>
+        <v>0.200838108426977</v>
       </c>
     </row>
     <row r="73">
@@ -2543,16 +2543,16 @@
         </is>
       </c>
       <c r="B73" s="0" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C73" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D73" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E73" s="0" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="F73" s="0" t="inlineStr">
         <is>
@@ -2560,10 +2560,10 @@
         </is>
       </c>
       <c r="G73" s="0" t="n">
-        <v>0.1917782300424008</v>
+        <v>0.9046564873107019</v>
       </c>
       <c r="H73" s="0" t="n">
-        <v>1.062111722117706</v>
+        <v>0.2960193114600882</v>
       </c>
     </row>
     <row r="74">
@@ -2573,27 +2573,27 @@
         </is>
       </c>
       <c r="B74" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C74" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D74" s="0" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="E74" s="0" t="n">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="F74" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>6month charter</t>
         </is>
       </c>
       <c r="G74" s="0" t="n">
-        <v>0.1917782300424008</v>
+        <v>0.9037947824504795</v>
       </c>
       <c r="H74" s="0" t="n">
-        <v>1.062111722117706</v>
+        <v>0.1795610746328801</v>
       </c>
     </row>
     <row r="75">
@@ -2603,27 +2603,27 @@
         </is>
       </c>
       <c r="B75" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C75" s="0" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D75" s="0" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="E75" s="0" t="n">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="F75" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>6month charter</t>
         </is>
       </c>
       <c r="G75" s="0" t="n">
-        <v>0.1917782300424008</v>
+        <v>0.9037947824504795</v>
       </c>
       <c r="H75" s="0" t="n">
-        <v>1.062111722117706</v>
+        <v>0.1795610746328801</v>
       </c>
     </row>
     <row r="76">
@@ -2636,24 +2636,24 @@
         <v>0</v>
       </c>
       <c r="C76" s="0" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="D76" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="E76" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="E76" s="0" t="n">
-        <v>800</v>
-      </c>
       <c r="F76" s="0" t="inlineStr">
         <is>
           <t>6month charter</t>
         </is>
       </c>
       <c r="G76" s="0" t="n">
-        <v>0.1854310109720958</v>
+        <v>0.9037947824504795</v>
       </c>
       <c r="H76" s="0" t="n">
-        <v>1.010016679772883</v>
+        <v>0.1795610746328801</v>
       </c>
     </row>
     <row r="77">
@@ -2663,27 +2663,27 @@
         </is>
       </c>
       <c r="B77" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C77" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="E77" s="0" t="n">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="F77" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>6month charter</t>
         </is>
       </c>
       <c r="G77" s="0" t="n">
-        <v>0.1819513182163064</v>
+        <v>0.9037947824504795</v>
       </c>
       <c r="H77" s="0" t="n">
-        <v>1.027681741557862</v>
+        <v>0.1795610746328801</v>
       </c>
     </row>
     <row r="78">
@@ -2693,27 +2693,27 @@
         </is>
       </c>
       <c r="B78" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C78" s="0" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="E78" s="0" t="n">
         <v>600</v>
       </c>
       <c r="F78" s="0" t="inlineStr">
         <is>
-          <t>3month charter</t>
+          <t>6month charter</t>
         </is>
       </c>
       <c r="G78" s="0" t="n">
-        <v>0.157249784248493</v>
+        <v>0.9037947824504795</v>
       </c>
       <c r="H78" s="0" t="n">
-        <v>0.9922860926842825</v>
+        <v>0.1795610746328801</v>
       </c>
     </row>
     <row r="79">
@@ -2723,27 +2723,27 @@
         </is>
       </c>
       <c r="B79" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C79" s="0" t="n">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="E79" s="0" t="n">
         <v>600</v>
       </c>
       <c r="F79" s="0" t="inlineStr">
         <is>
-          <t>3month charter</t>
+          <t>6month charter</t>
         </is>
       </c>
       <c r="G79" s="0" t="n">
-        <v>0.157249784248493</v>
+        <v>0.9037947824504795</v>
       </c>
       <c r="H79" s="0" t="n">
-        <v>0.9922860926842825</v>
+        <v>0.1795610746328801</v>
       </c>
     </row>
     <row r="80">
@@ -2753,16 +2753,16 @@
         </is>
       </c>
       <c r="B80" s="0" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C80" s="0" t="n">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="D80" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E80" s="0" t="n">
-        <v>600</v>
+        <v>1300</v>
       </c>
       <c r="F80" s="0" t="inlineStr">
         <is>
@@ -2770,10 +2770,10 @@
         </is>
       </c>
       <c r="G80" s="0" t="n">
-        <v>0.157249784248493</v>
+        <v>0.7476573351765203</v>
       </c>
       <c r="H80" s="0" t="n">
-        <v>0.9922860926842825</v>
+        <v>0.1277121906606214</v>
       </c>
     </row>
     <row r="81">
@@ -2783,27 +2783,27 @@
         </is>
       </c>
       <c r="B81" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="C81" s="0" t="n">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E81" s="0" t="n">
-        <v>700</v>
+        <v>1500</v>
       </c>
       <c r="F81" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>3month charter</t>
         </is>
       </c>
       <c r="G81" s="0" t="n">
-        <v>0.1230255922012378</v>
+        <v>0.7476573351765203</v>
       </c>
       <c r="H81" s="0" t="n">
-        <v>0.9048913295042762</v>
+        <v>0.1277121906606214</v>
       </c>
     </row>
     <row r="82">
@@ -2813,27 +2813,27 @@
         </is>
       </c>
       <c r="B82" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="C82" s="0" t="n">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="D82" s="0" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E82" s="0" t="n">
-        <v>700</v>
+        <v>1500</v>
       </c>
       <c r="F82" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>3month charter</t>
         </is>
       </c>
       <c r="G82" s="0" t="n">
-        <v>0.1230255922012378</v>
+        <v>0.7476573351765203</v>
       </c>
       <c r="H82" s="0" t="n">
-        <v>0.9048913295042762</v>
+        <v>0.1277121906606214</v>
       </c>
     </row>
     <row r="83">
@@ -2843,27 +2843,27 @@
         </is>
       </c>
       <c r="B83" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="C83" s="0" t="n">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="D83" s="0" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E83" s="0" t="n">
-        <v>700</v>
+        <v>1300</v>
       </c>
       <c r="F83" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>3month charter</t>
         </is>
       </c>
       <c r="G83" s="0" t="n">
-        <v>0.1230255922012378</v>
+        <v>0.7476573351765203</v>
       </c>
       <c r="H83" s="0" t="n">
-        <v>0.9048913295042762</v>
+        <v>0.1277121906606214</v>
       </c>
     </row>
     <row r="84">
@@ -2873,16 +2873,16 @@
         </is>
       </c>
       <c r="B84" s="0" t="n">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C84" s="0" t="n">
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="D84" s="0" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E84" s="0" t="n">
-        <v>650</v>
+        <v>1500</v>
       </c>
       <c r="F84" s="0" t="inlineStr">
         <is>
@@ -2890,10 +2890,10 @@
         </is>
       </c>
       <c r="G84" s="0" t="n">
-        <v>0.07440143306444946</v>
+        <v>0.7476573351765203</v>
       </c>
       <c r="H84" s="0" t="n">
-        <v>0.8931159990778167</v>
+        <v>0.1277121906606214</v>
       </c>
     </row>
     <row r="85">
@@ -2903,27 +2903,27 @@
         </is>
       </c>
       <c r="B85" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C85" s="0" t="n">
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="D85" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E85" s="0" t="n">
-        <v>650</v>
+        <v>1100</v>
       </c>
       <c r="F85" s="0" t="inlineStr">
         <is>
-          <t>3month charter</t>
+          <t>36month charter</t>
         </is>
       </c>
       <c r="G85" s="0" t="n">
-        <v>0.07440143306444946</v>
+        <v>0.7357630310543921</v>
       </c>
       <c r="H85" s="0" t="n">
-        <v>0.8931159990778167</v>
+        <v>0.07357264320187878</v>
       </c>
     </row>
     <row r="86">
@@ -2933,27 +2933,27 @@
         </is>
       </c>
       <c r="B86" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C86" s="0" t="n">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="D86" s="0" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E86" s="0" t="n">
-        <v>650</v>
+        <v>1500</v>
       </c>
       <c r="F86" s="0" t="inlineStr">
         <is>
-          <t>3month charter</t>
+          <t>36month charter</t>
         </is>
       </c>
       <c r="G86" s="0" t="n">
-        <v>0.0626948235405987</v>
+        <v>0.7357630310543921</v>
       </c>
       <c r="H86" s="0" t="n">
-        <v>0.8750345442358557</v>
+        <v>0.07357264320187878</v>
       </c>
     </row>
     <row r="87">
@@ -2963,27 +2963,27 @@
         </is>
       </c>
       <c r="B87" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C87" s="0" t="n">
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="D87" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E87" s="0" t="n">
-        <v>700</v>
+        <v>1500</v>
       </c>
       <c r="F87" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>36month charter</t>
         </is>
       </c>
       <c r="G87" s="0" t="n">
-        <v>0.0561959498849091</v>
+        <v>0.7357630310543921</v>
       </c>
       <c r="H87" s="0" t="n">
-        <v>0.8162516494270433</v>
+        <v>0.07357264320187878</v>
       </c>
     </row>
     <row r="88">
@@ -2993,27 +2993,27 @@
         </is>
       </c>
       <c r="B88" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C88" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D88" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E88" s="0" t="n">
-        <v>650</v>
+        <v>1100</v>
       </c>
       <c r="F88" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>36month charter</t>
         </is>
       </c>
       <c r="G88" s="0" t="n">
-        <v>0.05234991781459647</v>
+        <v>0.7357630310543921</v>
       </c>
       <c r="H88" s="0" t="n">
-        <v>0.7709809797032198</v>
+        <v>0.07357264320187878</v>
       </c>
     </row>
     <row r="89">
@@ -3023,27 +3023,27 @@
         </is>
       </c>
       <c r="B89" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C89" s="0" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D89" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E89" s="0" t="n">
-        <v>650</v>
+        <v>1500</v>
       </c>
       <c r="F89" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>36month charter</t>
         </is>
       </c>
       <c r="G89" s="0" t="n">
-        <v>0.05234991781459647</v>
+        <v>0.7357630310543921</v>
       </c>
       <c r="H89" s="0" t="n">
-        <v>0.7709809797032198</v>
+        <v>0.07357264320187878</v>
       </c>
     </row>
     <row r="90">
@@ -3053,27 +3053,27 @@
         </is>
       </c>
       <c r="B90" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C90" s="0" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="D90" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E90" s="0" t="n">
-        <v>650</v>
+        <v>800</v>
       </c>
       <c r="F90" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>36month charter</t>
         </is>
       </c>
       <c r="G90" s="0" t="n">
-        <v>0.05234991781459647</v>
+        <v>0.7357630310543921</v>
       </c>
       <c r="H90" s="0" t="n">
-        <v>0.7709809797032198</v>
+        <v>0.07357264320187878</v>
       </c>
     </row>
     <row r="91">
@@ -3083,27 +3083,27 @@
         </is>
       </c>
       <c r="B91" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C91" s="0" t="n">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="D91" s="0" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E91" s="0" t="n">
-        <v>650</v>
+        <v>1100</v>
       </c>
       <c r="F91" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>36month charter</t>
         </is>
       </c>
       <c r="G91" s="0" t="n">
-        <v>0.05234991781459647</v>
+        <v>0.7357630310543921</v>
       </c>
       <c r="H91" s="0" t="n">
-        <v>0.7709809797032198</v>
+        <v>0.07357264320187878</v>
       </c>
     </row>
     <row r="92">
@@ -3113,27 +3113,27 @@
         </is>
       </c>
       <c r="B92" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C92" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D92" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E92" s="0" t="n">
-        <v>650</v>
+        <v>1100</v>
       </c>
       <c r="F92" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>36month charter</t>
         </is>
       </c>
       <c r="G92" s="0" t="n">
-        <v>0.05234991781459647</v>
+        <v>0.7357630310543921</v>
       </c>
       <c r="H92" s="0" t="n">
-        <v>0.7709809797032198</v>
+        <v>0.07357264320187878</v>
       </c>
     </row>
     <row r="93">
@@ -3143,27 +3143,27 @@
         </is>
       </c>
       <c r="B93" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C93" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D93" s="0" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E93" s="0" t="n">
-        <v>650</v>
+        <v>1100</v>
       </c>
       <c r="F93" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>36month charter</t>
         </is>
       </c>
       <c r="G93" s="0" t="n">
-        <v>0.05234991781459647</v>
+        <v>0.7357630310543921</v>
       </c>
       <c r="H93" s="0" t="n">
-        <v>0.7709809797032198</v>
+        <v>0.07357264320187878</v>
       </c>
     </row>
     <row r="94">
@@ -3173,27 +3173,27 @@
         </is>
       </c>
       <c r="B94" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C94" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D94" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E94" s="0" t="n">
-        <v>650</v>
+        <v>1100</v>
       </c>
       <c r="F94" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>36month charter</t>
         </is>
       </c>
       <c r="G94" s="0" t="n">
-        <v>0.05234991781459647</v>
+        <v>0.7357630310543921</v>
       </c>
       <c r="H94" s="0" t="n">
-        <v>0.7709809797032198</v>
+        <v>0.07357264320187878</v>
       </c>
     </row>
     <row r="95">
@@ -3203,27 +3203,27 @@
         </is>
       </c>
       <c r="B95" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C95" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D95" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E95" s="0" t="n">
-        <v>650</v>
+        <v>1100</v>
       </c>
       <c r="F95" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>36month charter</t>
         </is>
       </c>
       <c r="G95" s="0" t="n">
-        <v>0.05234991781459647</v>
+        <v>0.7357630310543921</v>
       </c>
       <c r="H95" s="0" t="n">
-        <v>0.7709809797032198</v>
+        <v>0.07357264320187878</v>
       </c>
     </row>
     <row r="96">
@@ -3233,27 +3233,27 @@
         </is>
       </c>
       <c r="B96" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C96" s="0" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="D96" s="0" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="E96" s="0" t="n">
-        <v>1100</v>
+        <v>1500</v>
       </c>
       <c r="F96" s="0" t="inlineStr">
         <is>
-          <t>3month charter</t>
+          <t>36month charter</t>
         </is>
       </c>
       <c r="G96" s="0" t="n">
-        <v>0.03994961675896671</v>
+        <v>0.7357630310543921</v>
       </c>
       <c r="H96" s="0" t="n">
-        <v>0.8187181500282272</v>
+        <v>0.07357264320187878</v>
       </c>
     </row>
     <row r="97">
@@ -3263,27 +3263,27 @@
         </is>
       </c>
       <c r="B97" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C97" s="0" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D97" s="0" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="E97" s="0" t="n">
         <v>1100</v>
       </c>
       <c r="F97" s="0" t="inlineStr">
         <is>
-          <t>3month charter</t>
+          <t>36month charter</t>
         </is>
       </c>
       <c r="G97" s="0" t="n">
-        <v>0.03994961675896671</v>
+        <v>0.7357630310543921</v>
       </c>
       <c r="H97" s="0" t="n">
-        <v>0.8187181500282272</v>
+        <v>0.07357264320187878</v>
       </c>
     </row>
     <row r="98">
@@ -3293,27 +3293,27 @@
         </is>
       </c>
       <c r="B98" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C98" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D98" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E98" s="0" t="n">
-        <v>1100</v>
+        <v>1500</v>
       </c>
       <c r="F98" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>36month charter</t>
         </is>
       </c>
       <c r="G98" s="0" t="n">
-        <v>0.03188793754061878</v>
+        <v>0.7357630310543921</v>
       </c>
       <c r="H98" s="0" t="n">
-        <v>0.6696282024821837</v>
+        <v>0.07357264320187878</v>
       </c>
     </row>
     <row r="99">
@@ -3323,16 +3323,16 @@
         </is>
       </c>
       <c r="B99" s="0" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C99" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D99" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E99" s="0" t="n">
-        <v>1300</v>
+        <v>800</v>
       </c>
       <c r="F99" s="0" t="inlineStr">
         <is>
@@ -3340,10 +3340,10 @@
         </is>
       </c>
       <c r="G99" s="0" t="n">
-        <v>0.03089774180981113</v>
+        <v>0.7291162015662974</v>
       </c>
       <c r="H99" s="0" t="n">
-        <v>0.6632821852441134</v>
+        <v>0.1212965293460148</v>
       </c>
     </row>
     <row r="100">
@@ -3353,27 +3353,27 @@
         </is>
       </c>
       <c r="B100" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C100" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D100" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E100" s="0" t="n">
-        <v>1300</v>
+        <v>650</v>
       </c>
       <c r="F100" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>36month charter</t>
         </is>
       </c>
       <c r="G100" s="0" t="n">
-        <v>0.03089774180981113</v>
+        <v>0.7203397331870348</v>
       </c>
       <c r="H100" s="0" t="n">
-        <v>0.6632821852441134</v>
+        <v>0.08217743755743591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename variables and constans which is relaterd to action charter.
</commit_message>
<xml_diff>
--- a/output/ship_rule_charter.xlsx
+++ b/output/ship_rule_charter.xlsx
@@ -383,33 +383,33 @@
         </is>
       </c>
       <c r="B1" s="0" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C1" s="0" t="n">
         <v>60</v>
       </c>
       <c r="D1" s="0" t="n">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="E1" s="0" t="n">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="F1" s="0" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G1" s="0" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="H1" s="0" t="inlineStr">
         <is>
-          <t>3month charter, 10 ships</t>
+          <t>36month charter, 2 ships</t>
         </is>
       </c>
       <c r="I1" s="0" t="n">
-        <v>0.1945983865522247</v>
+        <v>0.1110535192194497</v>
       </c>
       <c r="J1" s="0" t="n">
-        <v>0.1097037938130009</v>
+        <v>0.09471664861170863</v>
       </c>
     </row>
     <row r="2">
@@ -419,33 +419,33 @@
         </is>
       </c>
       <c r="B2" s="0" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>60</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="H2" s="0" t="inlineStr">
         <is>
-          <t>3month charter, 10 ships</t>
+          <t>36month charter, 2 ships</t>
         </is>
       </c>
       <c r="I2" s="0" t="n">
-        <v>0.1945983865522247</v>
+        <v>0.1110535192194497</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>0.1097037938130009</v>
+        <v>0.09471664861170863</v>
       </c>
     </row>
     <row r="3">
@@ -455,33 +455,33 @@
         </is>
       </c>
       <c r="B3" s="0" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>60</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="H3" s="0" t="inlineStr">
         <is>
-          <t>3month charter, 10 ships</t>
+          <t>36month charter, 2 ships</t>
         </is>
       </c>
       <c r="I3" s="0" t="n">
-        <v>0.1945983865522247</v>
+        <v>0.1110535192194497</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>0.1097037938130009</v>
+        <v>0.09471664861170863</v>
       </c>
     </row>
     <row r="4">
@@ -491,33 +491,33 @@
         </is>
       </c>
       <c r="B4" s="0" t="n">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="H4" s="0" t="inlineStr">
         <is>
-          <t>3month charter, 10 ships</t>
+          <t>36month charter, 4 ships</t>
         </is>
       </c>
       <c r="I4" s="0" t="n">
-        <v>0.1945983865522247</v>
+        <v>-0.07413440137386836</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>0.1097037938130009</v>
+        <v>0.08081411992475478</v>
       </c>
     </row>
     <row r="5">
@@ -527,33 +527,33 @@
         </is>
       </c>
       <c r="B5" s="0" t="n">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="H5" s="0" t="inlineStr">
         <is>
-          <t>3month charter, 10 ships</t>
+          <t>36month charter, 4 ships</t>
         </is>
       </c>
       <c r="I5" s="0" t="n">
-        <v>0.1931194592613442</v>
+        <v>-0.07413440137386836</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>0.1087320144538868</v>
+        <v>0.08081411992475478</v>
       </c>
     </row>
     <row r="6">
@@ -563,33 +563,33 @@
         </is>
       </c>
       <c r="B6" s="0" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="H6" s="0" t="inlineStr">
         <is>
-          <t>3month charter, 15 ships</t>
+          <t>6month charter, 15 ships</t>
         </is>
       </c>
       <c r="I6" s="0" t="n">
-        <v>0.1606140123388825</v>
+        <v>-0.1193614173823362</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>0.1040678916100266</v>
+        <v>0.08405506722272815</v>
       </c>
     </row>
     <row r="7">
@@ -599,33 +599,33 @@
         </is>
       </c>
       <c r="B7" s="0" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>150</v>
       </c>
       <c r="H7" s="0" t="inlineStr">
         <is>
-          <t>3month charter, 15 ships</t>
+          <t>12month charter, 25 ships</t>
         </is>
       </c>
       <c r="I7" s="0" t="n">
-        <v>0.1606140123388825</v>
+        <v>-0.2500398673130042</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>0.1040678916100266</v>
+        <v>0.04424941480397088</v>
       </c>
     </row>
     <row r="8">
@@ -638,30 +638,30 @@
         <v>60</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="H8" s="0" t="inlineStr">
         <is>
-          <t>3month charter, 15 ships</t>
+          <t>36month charter, 4 ships</t>
         </is>
       </c>
       <c r="I8" s="0" t="n">
-        <v>0.1606140123388825</v>
+        <v>-0.2507070236846359</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>0.1040678916100266</v>
+        <v>0.04459498588584898</v>
       </c>
     </row>
     <row r="9">
@@ -671,33 +671,33 @@
         </is>
       </c>
       <c r="B9" s="0" t="n">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="H9" s="0" t="inlineStr">
         <is>
-          <t>3month charter, 10 ships</t>
+          <t>36month charter, 4 ships</t>
         </is>
       </c>
       <c r="I9" s="0" t="n">
-        <v>0.1210309455079945</v>
+        <v>-0.2507070236846359</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>0.1260472015917866</v>
+        <v>0.04459498588584898</v>
       </c>
     </row>
     <row r="10">
@@ -710,30 +710,30 @@
         <v>60</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="H10" s="0" t="inlineStr">
         <is>
-          <t>3month charter, 5 ships</t>
+          <t>36month charter, 4 ships</t>
         </is>
       </c>
       <c r="I10" s="0" t="n">
-        <v>0.1042576092661913</v>
+        <v>-0.2507070236846359</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>0.1123497934505275</v>
+        <v>0.04459498588584898</v>
       </c>
     </row>
     <row r="11">
@@ -743,33 +743,33 @@
         </is>
       </c>
       <c r="B11" s="0" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>1000</v>
+        <v>1800</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="H11" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 10 ships</t>
+          <t>3month charter, 5 ships</t>
         </is>
       </c>
       <c r="I11" s="0" t="n">
-        <v>0.06727993555947658</v>
+        <v>-0.2653780186356997</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>0.1139038462663897</v>
+        <v>0.05264426309571655</v>
       </c>
     </row>
     <row r="12">
@@ -779,33 +779,33 @@
         </is>
       </c>
       <c r="B12" s="0" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="H12" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 10 ships</t>
+          <t>3month charter, 5 ships</t>
         </is>
       </c>
       <c r="I12" s="0" t="n">
-        <v>0.06727993555947658</v>
+        <v>-0.2653780186356997</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>0.1139038462663897</v>
+        <v>0.05264426309571655</v>
       </c>
     </row>
     <row r="13">
@@ -815,33 +815,33 @@
         </is>
       </c>
       <c r="B13" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C13" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>1400</v>
+      </c>
+      <c r="F13" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="D13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>100</v>
-      </c>
       <c r="G13" s="0" t="n">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="H13" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 10 ships</t>
+          <t>3month charter, 3 ships</t>
         </is>
       </c>
       <c r="I13" s="0" t="n">
-        <v>0.06727993555947658</v>
+        <v>-0.3158717603812074</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>0.1139038462663897</v>
+        <v>0.09040928949888978</v>
       </c>
     </row>
     <row r="14">
@@ -851,33 +851,33 @@
         </is>
       </c>
       <c r="B14" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>1400</v>
+      </c>
+      <c r="F14" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="C14" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>90</v>
-      </c>
       <c r="G14" s="0" t="n">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="H14" s="0" t="inlineStr">
         <is>
-          <t>3month charter, 15 ships</t>
+          <t>3month charter, 3 ships</t>
         </is>
       </c>
       <c r="I14" s="0" t="n">
-        <v>-0.07030626888575287</v>
+        <v>-0.3158717603812074</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>0.09961441141170109</v>
+        <v>0.09040928949888978</v>
       </c>
     </row>
     <row r="15">
@@ -887,33 +887,33 @@
         </is>
       </c>
       <c r="B15" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>1400</v>
+      </c>
+      <c r="F15" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="C15" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <v>90</v>
-      </c>
       <c r="G15" s="0" t="n">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="H15" s="0" t="inlineStr">
         <is>
-          <t>3month charter, 15 ships</t>
+          <t>3month charter, 3 ships</t>
         </is>
       </c>
       <c r="I15" s="0" t="n">
-        <v>-0.07030626888575287</v>
+        <v>-0.3158717603812074</v>
       </c>
       <c r="J15" s="0" t="n">
-        <v>0.09961441141170109</v>
+        <v>0.09040928949888978</v>
       </c>
     </row>
     <row r="16">
@@ -923,33 +923,33 @@
         </is>
       </c>
       <c r="B16" s="0" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="H16" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 10 ships</t>
+          <t>6month charter, 4 ships</t>
         </is>
       </c>
       <c r="I16" s="0" t="n">
-        <v>-0.2364511146898293</v>
+        <v>-0.3194571319169012</v>
       </c>
       <c r="J16" s="0" t="n">
-        <v>0.03759820521992559</v>
+        <v>0.08975079045353825</v>
       </c>
     </row>
     <row r="17">
@@ -959,33 +959,33 @@
         </is>
       </c>
       <c r="B17" s="0" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>1800</v>
+        <v>1100</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="H17" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 10 ships</t>
+          <t>3month charter, 5 ships</t>
         </is>
       </c>
       <c r="I17" s="0" t="n">
-        <v>-0.2697979966506988</v>
+        <v>-0.3195060874799664</v>
       </c>
       <c r="J17" s="0" t="n">
-        <v>0.05523805818984528</v>
+        <v>0.08978968118346921</v>
       </c>
     </row>
     <row r="18">
@@ -995,33 +995,33 @@
         </is>
       </c>
       <c r="B18" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>1800</v>
+        <v>1500</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="H18" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 10 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I18" s="0" t="n">
-        <v>-0.2697979966506988</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J18" s="0" t="n">
-        <v>0.05523805818984528</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="19">
@@ -1040,24 +1040,24 @@
         <v>0</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>900</v>
+        <v>500</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>80</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>110</v>
+        <v>200</v>
       </c>
       <c r="H19" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 10 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I19" s="0" t="n">
-        <v>-0.2812653288942285</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J19" s="0" t="n">
-        <v>0.06233185322122759</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="20">
@@ -1067,33 +1067,33 @@
         </is>
       </c>
       <c r="B20" s="0" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C20" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>1300</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F20" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="D20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="0" t="n">
-        <v>900</v>
-      </c>
-      <c r="F20" s="0" t="n">
-        <v>80</v>
-      </c>
       <c r="G20" s="0" t="n">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="H20" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 10 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I20" s="0" t="n">
-        <v>-0.2812653288942285</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J20" s="0" t="n">
-        <v>0.06233185322122759</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="21">
@@ -1103,33 +1103,33 @@
         </is>
       </c>
       <c r="B21" s="0" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C21" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1300</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F21" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="D21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>900</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>80</v>
-      </c>
       <c r="G21" s="0" t="n">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="H21" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 10 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I21" s="0" t="n">
-        <v>-0.2812653288942285</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J21" s="0" t="n">
-        <v>0.06233185322122759</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="22">
@@ -1139,33 +1139,33 @@
         </is>
       </c>
       <c r="B22" s="0" t="n">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>900</v>
+        <v>1000</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="H22" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 10 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I22" s="0" t="n">
-        <v>-0.2812653288942285</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J22" s="0" t="n">
-        <v>0.06233185322122759</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="23">
@@ -1175,33 +1175,33 @@
         </is>
       </c>
       <c r="B23" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C23" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>1100</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="D23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" s="0" t="n">
-        <v>900</v>
-      </c>
-      <c r="F23" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="G23" s="0" t="n">
-        <v>110</v>
-      </c>
       <c r="H23" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 10 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I23" s="0" t="n">
-        <v>-0.2812653288942285</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J23" s="0" t="n">
-        <v>0.06233185322122759</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="24">
@@ -1220,24 +1220,24 @@
         <v>0</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>900</v>
+        <v>500</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>80</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>110</v>
+        <v>200</v>
       </c>
       <c r="H24" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 10 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I24" s="0" t="n">
-        <v>-0.2812653288942285</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J24" s="0" t="n">
-        <v>0.06233185322122759</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="25">
@@ -1247,33 +1247,33 @@
         </is>
       </c>
       <c r="B25" s="0" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="H25" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 100 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I25" s="0" t="n">
-        <v>-0.2963576791362938</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J25" s="0" t="n">
-        <v>0.07246981310391497</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="26">
@@ -1283,33 +1283,33 @@
         </is>
       </c>
       <c r="B26" s="0" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>160</v>
+        <v>105</v>
       </c>
       <c r="H26" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 100 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I26" s="0" t="n">
-        <v>-0.2963576791362938</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J26" s="0" t="n">
-        <v>0.07246981310391497</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="27">
@@ -1319,33 +1319,33 @@
         </is>
       </c>
       <c r="B27" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C27" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="C27" s="0" t="n">
-        <v>90</v>
-      </c>
       <c r="D27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="E27" s="0" t="n">
-        <v>1000</v>
-      </c>
       <c r="F27" s="0" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H27" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 100 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I27" s="0" t="n">
-        <v>-0.2963576791362938</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J27" s="0" t="n">
-        <v>0.07246981310391497</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="28">
@@ -1355,33 +1355,33 @@
         </is>
       </c>
       <c r="B28" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>1300</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F28" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="C28" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="D28" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="E28" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F28" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="G28" s="0" t="n">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="H28" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 100 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I28" s="0" t="n">
-        <v>-0.2963576791362938</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J28" s="0" t="n">
-        <v>0.07246981310391497</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="29">
@@ -1391,33 +1391,33 @@
         </is>
       </c>
       <c r="B29" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="H29" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 100 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I29" s="0" t="n">
-        <v>-0.3003016309244051</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J29" s="0" t="n">
-        <v>0.07526923393916639</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="30">
@@ -1427,33 +1427,33 @@
         </is>
       </c>
       <c r="B30" s="0" t="n">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>90</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>600</v>
+        <v>800</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="H30" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 100 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I30" s="0" t="n">
-        <v>-0.3003016309244051</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J30" s="0" t="n">
-        <v>0.07526923393916639</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="31">
@@ -1463,33 +1463,33 @@
         </is>
       </c>
       <c r="B31" s="0" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="H31" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I31" s="0" t="n">
-        <v>-0.3106916244054833</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J31" s="0" t="n">
-        <v>0.08294192066626968</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="32">
@@ -1499,33 +1499,33 @@
         </is>
       </c>
       <c r="B32" s="0" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>1000</v>
+        <v>1800</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>90</v>
+        <v>160</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="H32" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I32" s="0" t="n">
-        <v>-0.3106916244054833</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J32" s="0" t="n">
-        <v>0.08294192066626968</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="33">
@@ -1535,33 +1535,33 @@
         </is>
       </c>
       <c r="B33" s="0" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F33" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="G33" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="G33" s="0" t="n">
-        <v>150</v>
-      </c>
       <c r="H33" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I33" s="0" t="n">
-        <v>-0.3106916244054833</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J33" s="0" t="n">
-        <v>0.08294192066626968</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="34">
@@ -1571,33 +1571,33 @@
         </is>
       </c>
       <c r="B34" s="0" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>1000</v>
+        <v>1800</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>90</v>
+        <v>160</v>
       </c>
       <c r="G34" s="0" t="n">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="H34" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I34" s="0" t="n">
-        <v>-0.3106916244054833</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J34" s="0" t="n">
-        <v>0.08294192066626968</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="35">
@@ -1607,33 +1607,33 @@
         </is>
       </c>
       <c r="B35" s="0" t="n">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>1000</v>
+        <v>1300</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G35" s="0" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="H35" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>6month charter, 100 ships</t>
         </is>
       </c>
       <c r="I35" s="0" t="n">
-        <v>-0.3106916244054833</v>
+        <v>-0.4585047099065456</v>
       </c>
       <c r="J35" s="0" t="n">
-        <v>0.08294192066626968</v>
+        <v>0.05090856287397438</v>
       </c>
     </row>
     <row r="36">
@@ -1643,33 +1643,33 @@
         </is>
       </c>
       <c r="B36" s="0" t="n">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>1000</v>
+        <v>1300</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G36" s="0" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="H36" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>6month charter, 100 ships</t>
         </is>
       </c>
       <c r="I36" s="0" t="n">
-        <v>-0.3106916244054833</v>
+        <v>-0.4585047099065456</v>
       </c>
       <c r="J36" s="0" t="n">
-        <v>0.08294192066626968</v>
+        <v>0.05090856287397438</v>
       </c>
     </row>
     <row r="37">
@@ -1679,33 +1679,33 @@
         </is>
       </c>
       <c r="B37" s="0" t="n">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>1000</v>
+        <v>1300</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G37" s="0" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="H37" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>6month charter, 100 ships</t>
         </is>
       </c>
       <c r="I37" s="0" t="n">
-        <v>-0.3106916244054833</v>
+        <v>-0.4585047099065456</v>
       </c>
       <c r="J37" s="0" t="n">
-        <v>0.08294192066626968</v>
+        <v>0.05090856287397438</v>
       </c>
     </row>
     <row r="38">
@@ -1715,33 +1715,33 @@
         </is>
       </c>
       <c r="B38" s="0" t="n">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="E38" s="0" t="n">
-        <v>1000</v>
+        <v>1300</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G38" s="0" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="H38" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>6month charter, 100 ships</t>
         </is>
       </c>
       <c r="I38" s="0" t="n">
-        <v>-0.3106916244054833</v>
+        <v>-0.4585047099065456</v>
       </c>
       <c r="J38" s="0" t="n">
-        <v>0.08294192066626968</v>
+        <v>0.05090856287397438</v>
       </c>
     </row>
     <row r="39">
@@ -1751,33 +1751,33 @@
         </is>
       </c>
       <c r="B39" s="0" t="n">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>800</v>
+        <v>1400</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="G39" s="0" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="H39" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I39" s="0" t="n">
-        <v>-0.3106916244054833</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J39" s="0" t="n">
-        <v>0.08294192066626968</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="40">
@@ -1787,33 +1787,33 @@
         </is>
       </c>
       <c r="B40" s="0" t="n">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>800</v>
+        <v>1400</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="G40" s="0" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="H40" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I40" s="0" t="n">
-        <v>-0.3106916244054833</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J40" s="0" t="n">
-        <v>0.08294192066626968</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="41">
@@ -1823,33 +1823,33 @@
         </is>
       </c>
       <c r="B41" s="0" t="n">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>800</v>
+        <v>1100</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="G41" s="0" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="H41" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
       <c r="I41" s="0" t="n">
-        <v>-0.3106916244054833</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="J41" s="0" t="n">
-        <v>0.08294192066626968</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="42">
@@ -1859,33 +1859,33 @@
         </is>
       </c>
       <c r="B42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" s="0" t="n">
         <v>60</v>
-      </c>
-      <c r="C42" s="0" t="n">
-        <v>70</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>800</v>
       </c>
       <c r="E42" s="0" t="n">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="G42" s="0" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="H42" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>36month charter, 100 ships</t>
         </is>
       </c>
       <c r="I42" s="0" t="n">
-        <v>-0.3106916244054833</v>
+        <v>-0.4655651795425902</v>
       </c>
       <c r="J42" s="0" t="n">
-        <v>0.08294192066626968</v>
+        <v>0.03178222300504591</v>
       </c>
     </row>
     <row r="43">
@@ -1895,22 +1895,22 @@
         </is>
       </c>
       <c r="B43" s="0" t="n">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E43" s="0" t="n">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="G43" s="0" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="H43" s="0" t="inlineStr">
         <is>
@@ -1931,19 +1931,19 @@
         </is>
       </c>
       <c r="B44" s="0" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="E44" s="0" t="n">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="F44" s="0" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="G44" s="0" t="n">
         <v>160</v>
@@ -1967,22 +1967,22 @@
         </is>
       </c>
       <c r="B45" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="E45" s="0" t="n">
-        <v>1000</v>
+        <v>1800</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G45" s="0" t="n">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="H45" s="0" t="inlineStr">
         <is>
@@ -2006,19 +2006,19 @@
         <v>90</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>500</v>
+        <v>900</v>
       </c>
       <c r="E46" s="0" t="n">
-        <v>900</v>
+        <v>3000</v>
       </c>
       <c r="F46" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G46" s="0" t="n">
-        <v>160</v>
+        <v>105</v>
       </c>
       <c r="H46" s="0" t="inlineStr">
         <is>
@@ -2042,19 +2042,19 @@
         <v>90</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>500</v>
+        <v>900</v>
       </c>
       <c r="E47" s="0" t="n">
-        <v>800</v>
+        <v>3000</v>
       </c>
       <c r="F47" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G47" s="0" t="n">
-        <v>160</v>
+        <v>105</v>
       </c>
       <c r="H47" s="0" t="inlineStr">
         <is>
@@ -2075,22 +2075,22 @@
         </is>
       </c>
       <c r="B48" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>1300</v>
+        <v>0</v>
       </c>
       <c r="E48" s="0" t="n">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F48" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G48" s="0" t="n">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="H48" s="0" t="inlineStr">
         <is>
@@ -2098,10 +2098,10 @@
         </is>
       </c>
       <c r="I48" s="0" t="n">
-        <v>-0.3195876800850752</v>
+        <v>-0.2486559791615969</v>
       </c>
       <c r="J48" s="0" t="n">
-        <v>0.08985452037021779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -2111,19 +2111,19 @@
         </is>
       </c>
       <c r="B49" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>500</v>
+        <v>1100</v>
       </c>
       <c r="E49" s="0" t="n">
-        <v>1000</v>
+        <v>1800</v>
       </c>
       <c r="F49" s="0" t="n">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="G49" s="0" t="n">
         <v>160</v>
@@ -2134,10 +2134,10 @@
         </is>
       </c>
       <c r="I49" s="0" t="n">
-        <v>-0.3195876800850752</v>
+        <v>-0.2486559791615969</v>
       </c>
       <c r="J49" s="0" t="n">
-        <v>0.08985452037021779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -2147,22 +2147,22 @@
         </is>
       </c>
       <c r="B50" s="0" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>1200</v>
+        <v>700</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>1400</v>
       </c>
       <c r="F50" s="0" t="n">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="G50" s="0" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="H50" s="0" t="inlineStr">
         <is>
@@ -2170,10 +2170,10 @@
         </is>
       </c>
       <c r="I50" s="0" t="n">
-        <v>-0.3195876800850752</v>
+        <v>-0.2486559791615969</v>
       </c>
       <c r="J50" s="0" t="n">
-        <v>0.08985452037021779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -2183,22 +2183,22 @@
         </is>
       </c>
       <c r="B51" s="0" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="E51" s="0" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="F51" s="0" t="n">
         <v>50</v>
       </c>
       <c r="G51" s="0" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="H51" s="0" t="inlineStr">
         <is>
@@ -2206,10 +2206,10 @@
         </is>
       </c>
       <c r="I51" s="0" t="n">
-        <v>-0.3195876800850752</v>
+        <v>-0.2486559791615969</v>
       </c>
       <c r="J51" s="0" t="n">
-        <v>0.08985452037021779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -2219,22 +2219,22 @@
         </is>
       </c>
       <c r="B52" s="0" t="n">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>110</v>
+        <v>30</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="E52" s="0" t="n">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="F52" s="0" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="G52" s="0" t="n">
-        <v>160</v>
+        <v>95</v>
       </c>
       <c r="H52" s="0" t="inlineStr">
         <is>
@@ -2242,10 +2242,10 @@
         </is>
       </c>
       <c r="I52" s="0" t="n">
-        <v>-0.3195876800850752</v>
+        <v>-0.2486559791615969</v>
       </c>
       <c r="J52" s="0" t="n">
-        <v>0.08985452037021779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -2255,22 +2255,22 @@
         </is>
       </c>
       <c r="B53" s="0" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>1300</v>
+        <v>1000</v>
       </c>
       <c r="E53" s="0" t="n">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="F53" s="0" t="n">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="G53" s="0" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="H53" s="0" t="inlineStr">
         <is>
@@ -2278,10 +2278,10 @@
         </is>
       </c>
       <c r="I53" s="0" t="n">
-        <v>-0.3195876800850752</v>
+        <v>-0.2486559791615969</v>
       </c>
       <c r="J53" s="0" t="n">
-        <v>0.08985452037021779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -2291,22 +2291,22 @@
         </is>
       </c>
       <c r="B54" s="0" t="n">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>500</v>
+        <v>1100</v>
       </c>
       <c r="E54" s="0" t="n">
-        <v>1000</v>
+        <v>1300</v>
       </c>
       <c r="F54" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="G54" s="0" t="n">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="H54" s="0" t="inlineStr">
         <is>
@@ -2314,10 +2314,10 @@
         </is>
       </c>
       <c r="I54" s="0" t="n">
-        <v>-0.3195876800850752</v>
+        <v>-0.2486559791615969</v>
       </c>
       <c r="J54" s="0" t="n">
-        <v>0.08985452037021779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -2327,22 +2327,22 @@
         </is>
       </c>
       <c r="B55" s="0" t="n">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E55" s="0" t="n">
-        <v>1000</v>
+        <v>1800</v>
       </c>
       <c r="F55" s="0" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G55" s="0" t="n">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="H55" s="0" t="inlineStr">
         <is>
@@ -2350,10 +2350,10 @@
         </is>
       </c>
       <c r="I55" s="0" t="n">
-        <v>-0.3195876800850752</v>
+        <v>-0.2486559791615969</v>
       </c>
       <c r="J55" s="0" t="n">
-        <v>0.08985452037021779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -2363,22 +2363,22 @@
         </is>
       </c>
       <c r="B56" s="0" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="D56" s="0" t="n">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="E56" s="0" t="n">
-        <v>1000</v>
+        <v>1400</v>
       </c>
       <c r="F56" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G56" s="0" t="n">
-        <v>160</v>
+        <v>70</v>
       </c>
       <c r="H56" s="0" t="inlineStr">
         <is>
@@ -2386,10 +2386,10 @@
         </is>
       </c>
       <c r="I56" s="0" t="n">
-        <v>-0.3195876800850752</v>
+        <v>-0.2486559791615969</v>
       </c>
       <c r="J56" s="0" t="n">
-        <v>0.08985452037021779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -2399,22 +2399,22 @@
         </is>
       </c>
       <c r="B57" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="C57" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="C57" s="0" t="n">
-        <v>110</v>
-      </c>
       <c r="D57" s="0" t="n">
-        <v>500</v>
+        <v>900</v>
       </c>
       <c r="E57" s="0" t="n">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="F57" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G57" s="0" t="n">
-        <v>160</v>
+        <v>95</v>
       </c>
       <c r="H57" s="0" t="inlineStr">
         <is>
@@ -2422,10 +2422,10 @@
         </is>
       </c>
       <c r="I57" s="0" t="n">
-        <v>-0.3195876800850752</v>
+        <v>-0.2486559791615969</v>
       </c>
       <c r="J57" s="0" t="n">
-        <v>0.08985452037021779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -2435,33 +2435,33 @@
         </is>
       </c>
       <c r="B58" s="0" t="n">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="C58" s="0" t="n">
         <v>110</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E58" s="0" t="n">
-        <v>500</v>
+        <v>900</v>
       </c>
       <c r="F58" s="0" t="n">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="G58" s="0" t="n">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="H58" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>36month charter, 100 ships</t>
         </is>
       </c>
       <c r="I58" s="0" t="n">
-        <v>-0.3195876800850752</v>
+        <v>-0.3799236017326246</v>
       </c>
       <c r="J58" s="0" t="n">
-        <v>0.08985452037021779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -2471,33 +2471,33 @@
         </is>
       </c>
       <c r="B59" s="0" t="n">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D59" s="0" t="n">
         <v>500</v>
       </c>
       <c r="E59" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F59" s="0" t="n">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="G59" s="0" t="n">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="H59" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>36month charter, 100 ships</t>
         </is>
       </c>
       <c r="I59" s="0" t="n">
-        <v>-0.3195876800850752</v>
+        <v>-0.3799236017326246</v>
       </c>
       <c r="J59" s="0" t="n">
-        <v>0.08985452037021779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -2507,22 +2507,22 @@
         </is>
       </c>
       <c r="B60" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>500</v>
+        <v>1300</v>
       </c>
       <c r="E60" s="0" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="F60" s="0" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="G60" s="0" t="n">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="H60" s="0" t="inlineStr">
         <is>
@@ -2530,10 +2530,10 @@
         </is>
       </c>
       <c r="I60" s="0" t="n">
-        <v>-0.3195876800850752</v>
+        <v>-0.2486559791615969</v>
       </c>
       <c r="J60" s="0" t="n">
-        <v>0.08985452037021779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -2543,22 +2543,22 @@
         </is>
       </c>
       <c r="B61" s="0" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C61" s="0" t="n">
         <v>110</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="E61" s="0" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="F61" s="0" t="n">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="G61" s="0" t="n">
-        <v>160</v>
+        <v>105</v>
       </c>
       <c r="H61" s="0" t="inlineStr">
         <is>
@@ -2566,10 +2566,10 @@
         </is>
       </c>
       <c r="I61" s="0" t="n">
-        <v>-0.3195876800850752</v>
+        <v>-0.2486559791615969</v>
       </c>
       <c r="J61" s="0" t="n">
-        <v>0.08985452037021779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -2579,19 +2579,19 @@
         </is>
       </c>
       <c r="B62" s="0" t="n">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="C62" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="E62" s="0" t="n">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="F62" s="0" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G62" s="0" t="n">
         <v>150</v>
@@ -2602,10 +2602,10 @@
         </is>
       </c>
       <c r="I62" s="0" t="n">
-        <v>-0.3195876800850752</v>
+        <v>-0.2486559791615969</v>
       </c>
       <c r="J62" s="0" t="n">
-        <v>0.08985452037021779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -2615,22 +2615,22 @@
         </is>
       </c>
       <c r="B63" s="0" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>1300</v>
+        <v>300</v>
       </c>
       <c r="E63" s="0" t="n">
-        <v>1400</v>
+        <v>3000</v>
       </c>
       <c r="F63" s="0" t="n">
         <v>80</v>
       </c>
       <c r="G63" s="0" t="n">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H63" s="0" t="inlineStr">
         <is>
@@ -2638,10 +2638,10 @@
         </is>
       </c>
       <c r="I63" s="0" t="n">
-        <v>-0.3195876800850752</v>
+        <v>-0.2486559791615969</v>
       </c>
       <c r="J63" s="0" t="n">
-        <v>0.08985452037021779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -2651,22 +2651,22 @@
         </is>
       </c>
       <c r="B64" s="0" t="n">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="C64" s="0" t="n">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>1300</v>
+        <v>0</v>
       </c>
       <c r="E64" s="0" t="n">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="F64" s="0" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="G64" s="0" t="n">
-        <v>110</v>
+        <v>160</v>
       </c>
       <c r="H64" s="0" t="inlineStr">
         <is>
@@ -2674,10 +2674,10 @@
         </is>
       </c>
       <c r="I64" s="0" t="n">
-        <v>-0.3195876800850752</v>
+        <v>-0.2486559791615969</v>
       </c>
       <c r="J64" s="0" t="n">
-        <v>0.08985452037021779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -2687,22 +2687,22 @@
         </is>
       </c>
       <c r="B65" s="0" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="C65" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E65" s="0" t="n">
-        <v>1000</v>
+        <v>1300</v>
       </c>
       <c r="F65" s="0" t="n">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="G65" s="0" t="n">
-        <v>160</v>
+        <v>105</v>
       </c>
       <c r="H65" s="0" t="inlineStr">
         <is>
@@ -2710,10 +2710,10 @@
         </is>
       </c>
       <c r="I65" s="0" t="n">
-        <v>-0.3195876800850752</v>
+        <v>-0.2486559791615969</v>
       </c>
       <c r="J65" s="0" t="n">
-        <v>0.08985452037021779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -2723,33 +2723,33 @@
         </is>
       </c>
       <c r="B66" s="0" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C66" s="0" t="n">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E66" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F66" s="0" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="G66" s="0" t="n">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="H66" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>3month charter, 0 ships</t>
         </is>
       </c>
       <c r="I66" s="0" t="n">
-        <v>-0.3195876800850752</v>
+        <v>-0.2486559791615969</v>
       </c>
       <c r="J66" s="0" t="n">
-        <v>0.08985452037021779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">

</xml_diff>